<commit_message>
Add the player list and their overall
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="235">
   <si>
     <t>name</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>Byakuya Kuchiki</t>
-  </si>
-  <si>
-    <t>Midfileder</t>
   </si>
   <si>
     <t>bleach_8</t>
@@ -2679,18 +2676,18 @@
         <v>60</v>
       </c>
       <c r="H24" t="s" s="6">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="I24" t="s" s="6">
         <v>63</v>
       </c>
       <c r="J24" t="s" s="6">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="6">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="7">
         <v>0</v>
@@ -2717,12 +2714,12 @@
         <v>63</v>
       </c>
       <c r="J25" t="s" s="6">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="6">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="7">
         <v>11</v>
@@ -2749,12 +2746,12 @@
         <v>63</v>
       </c>
       <c r="J26" t="s" s="6">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" ht="32.05" customHeight="1">
       <c r="A27" t="s" s="6">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="7">
         <v>12</v>
@@ -2781,12 +2778,12 @@
         <v>63</v>
       </c>
       <c r="J27" t="s" s="6">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="6">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="7">
         <v>11</v>
@@ -2810,15 +2807,15 @@
         <v>11</v>
       </c>
       <c r="I28" t="s" s="6">
+        <v>74</v>
+      </c>
+      <c r="J28" t="s" s="6">
         <v>75</v>
-      </c>
-      <c r="J28" t="s" s="6">
-        <v>76</v>
       </c>
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="6">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="7">
         <v>6</v>
@@ -2842,15 +2839,15 @@
         <v>11</v>
       </c>
       <c r="I29" t="s" s="6">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J29" t="s" s="6">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="6">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="7">
         <v>6</v>
@@ -2874,15 +2871,15 @@
         <v>15</v>
       </c>
       <c r="I30" t="s" s="6">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J30" t="s" s="6">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" ht="32.05" customHeight="1">
       <c r="A31" t="s" s="6">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="7">
         <v>2</v>
@@ -2906,15 +2903,15 @@
         <v>15</v>
       </c>
       <c r="I31" t="s" s="6">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J31" t="s" s="6">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="6">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="7">
         <v>0</v>
@@ -2938,15 +2935,15 @@
         <v>15</v>
       </c>
       <c r="I32" t="s" s="6">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J32" t="s" s="6">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" ht="20.05" customHeight="1">
       <c r="A33" t="s" s="6">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="7">
         <v>0</v>
@@ -2970,15 +2967,15 @@
         <v>18</v>
       </c>
       <c r="I33" t="s" s="6">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J33" t="s" s="6">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" t="s" s="6">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" s="7">
         <v>14</v>
@@ -3002,15 +2999,15 @@
         <v>15</v>
       </c>
       <c r="I34" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="J34" t="s" s="6">
         <v>88</v>
-      </c>
-      <c r="J34" t="s" s="6">
-        <v>89</v>
       </c>
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" t="s" s="6">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" s="7">
         <v>23</v>
@@ -3034,15 +3031,15 @@
         <v>11</v>
       </c>
       <c r="I35" t="s" s="6">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J35" t="s" s="6">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" ht="32.05" customHeight="1">
       <c r="A36" t="s" s="6">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="7">
         <v>12</v>
@@ -3066,15 +3063,15 @@
         <v>15</v>
       </c>
       <c r="I36" t="s" s="6">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J36" t="s" s="6">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" t="s" s="6">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B37" s="7">
         <v>4</v>
@@ -3098,15 +3095,15 @@
         <v>18</v>
       </c>
       <c r="I37" t="s" s="6">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J37" t="s" s="6">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="6">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="7">
         <v>0</v>
@@ -3130,15 +3127,15 @@
         <v>18</v>
       </c>
       <c r="I38" t="s" s="6">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J38" t="s" s="6">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
       <c r="A39" t="s" s="6">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="7">
         <v>11</v>
@@ -3162,15 +3159,15 @@
         <v>11</v>
       </c>
       <c r="I39" t="s" s="6">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J39" t="s" s="6">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" t="s" s="6">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="7">
         <v>22</v>
@@ -3194,15 +3191,15 @@
         <v>15</v>
       </c>
       <c r="I40" t="s" s="6">
+        <v>100</v>
+      </c>
+      <c r="J40" t="s" s="6">
         <v>101</v>
-      </c>
-      <c r="J40" t="s" s="6">
-        <v>102</v>
       </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" t="s" s="6">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B41" s="7">
         <v>39</v>
@@ -3226,15 +3223,15 @@
         <v>11</v>
       </c>
       <c r="I41" t="s" s="6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J41" t="s" s="6">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" t="s" s="6">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B42" s="7">
         <v>16</v>
@@ -3255,18 +3252,18 @@
         <v>35</v>
       </c>
       <c r="H42" t="s" s="6">
+        <v>105</v>
+      </c>
+      <c r="I42" t="s" s="6">
+        <v>100</v>
+      </c>
+      <c r="J42" t="s" s="6">
         <v>106</v>
-      </c>
-      <c r="I42" t="s" s="6">
-        <v>101</v>
-      </c>
-      <c r="J42" t="s" s="6">
-        <v>107</v>
       </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="6">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B43" s="7">
         <v>8</v>
@@ -3290,15 +3287,15 @@
         <v>15</v>
       </c>
       <c r="I43" t="s" s="6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J43" t="s" s="6">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="6">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B44" s="7">
         <v>1</v>
@@ -3322,15 +3319,15 @@
         <v>18</v>
       </c>
       <c r="I44" t="s" s="6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J44" t="s" s="6">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" ht="20.05" customHeight="1">
       <c r="A45" t="s" s="6">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" s="7">
         <v>28</v>
@@ -3354,15 +3351,15 @@
         <v>11</v>
       </c>
       <c r="I45" t="s" s="6">
+        <v>112</v>
+      </c>
+      <c r="J45" t="s" s="6">
         <v>113</v>
-      </c>
-      <c r="J45" t="s" s="6">
-        <v>114</v>
       </c>
     </row>
     <row r="46" ht="20.05" customHeight="1">
       <c r="A46" t="s" s="6">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" s="7">
         <v>25</v>
@@ -3386,15 +3383,15 @@
         <v>11</v>
       </c>
       <c r="I46" t="s" s="6">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J46" t="s" s="6">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="6">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B47" s="7">
         <v>15</v>
@@ -3418,15 +3415,15 @@
         <v>15</v>
       </c>
       <c r="I47" t="s" s="6">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J47" t="s" s="6">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="6">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B48" s="7">
         <v>13</v>
@@ -3450,15 +3447,15 @@
         <v>15</v>
       </c>
       <c r="I48" t="s" s="6">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J48" t="s" s="6">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="6">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B49" s="7">
         <v>7</v>
@@ -3482,15 +3479,15 @@
         <v>15</v>
       </c>
       <c r="I49" t="s" s="6">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J49" t="s" s="6">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" t="s" s="6">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B50" s="7">
         <v>0</v>
@@ -3514,15 +3511,15 @@
         <v>18</v>
       </c>
       <c r="I50" t="s" s="6">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J50" t="s" s="6">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="6">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B51" s="7">
         <v>31</v>
@@ -3546,15 +3543,15 @@
         <v>11</v>
       </c>
       <c r="I51" t="s" s="6">
+        <v>125</v>
+      </c>
+      <c r="J51" t="s" s="6">
         <v>126</v>
-      </c>
-      <c r="J51" t="s" s="6">
-        <v>127</v>
       </c>
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="6">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B52" s="7">
         <v>32</v>
@@ -3578,15 +3575,15 @@
         <v>11</v>
       </c>
       <c r="I52" t="s" s="6">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J52" t="s" s="6">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="6">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B53" s="7">
         <v>7</v>
@@ -3610,15 +3607,15 @@
         <v>15</v>
       </c>
       <c r="I53" t="s" s="6">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J53" t="s" s="6">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" ht="20.05" customHeight="1">
       <c r="A54" t="s" s="6">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B54" s="7">
         <v>5</v>
@@ -3642,15 +3639,15 @@
         <v>15</v>
       </c>
       <c r="I54" t="s" s="6">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J54" t="s" s="6">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="6">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B55" s="7">
         <v>4</v>
@@ -3674,15 +3671,15 @@
         <v>18</v>
       </c>
       <c r="I55" t="s" s="6">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J55" t="s" s="6">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="6">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B56" s="7">
         <v>35</v>
@@ -3706,15 +3703,15 @@
         <v>11</v>
       </c>
       <c r="I56" t="s" s="6">
+        <v>136</v>
+      </c>
+      <c r="J56" t="s" s="6">
         <v>137</v>
-      </c>
-      <c r="J56" t="s" s="6">
-        <v>138</v>
       </c>
     </row>
     <row r="57" ht="20.05" customHeight="1">
       <c r="A57" t="s" s="6">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B57" s="7">
         <v>34</v>
@@ -3738,15 +3735,15 @@
         <v>11</v>
       </c>
       <c r="I57" t="s" s="6">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J57" t="s" s="6">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" ht="20.05" customHeight="1">
       <c r="A58" t="s" s="6">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B58" s="7">
         <v>14</v>
@@ -3770,15 +3767,15 @@
         <v>15</v>
       </c>
       <c r="I58" t="s" s="6">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J58" t="s" s="6">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" ht="20.05" customHeight="1">
       <c r="A59" t="s" s="6">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B59" s="7">
         <v>11</v>
@@ -3802,15 +3799,15 @@
         <v>32</v>
       </c>
       <c r="I59" t="s" s="6">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J59" t="s" s="6">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" ht="20.05" customHeight="1">
       <c r="A60" t="s" s="6">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B60" s="7">
         <v>5</v>
@@ -3834,15 +3831,15 @@
         <v>18</v>
       </c>
       <c r="I60" t="s" s="6">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J60" t="s" s="6">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" ht="20.05" customHeight="1">
       <c r="A61" t="s" s="6">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B61" s="7">
         <v>23</v>
@@ -3863,18 +3860,18 @@
         <v>64</v>
       </c>
       <c r="H61" t="s" s="6">
+        <v>147</v>
+      </c>
+      <c r="I61" t="s" s="6">
         <v>148</v>
       </c>
-      <c r="I61" t="s" s="6">
+      <c r="J61" t="s" s="6">
         <v>149</v>
-      </c>
-      <c r="J61" t="s" s="6">
-        <v>150</v>
       </c>
     </row>
     <row r="62" ht="20.05" customHeight="1">
       <c r="A62" t="s" s="6">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B62" s="7">
         <v>15</v>
@@ -3898,15 +3895,15 @@
         <v>15</v>
       </c>
       <c r="I62" t="s" s="6">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J62" t="s" s="6">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" ht="20.05" customHeight="1">
       <c r="A63" t="s" s="6">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B63" s="7">
         <v>13</v>
@@ -3930,15 +3927,15 @@
         <v>11</v>
       </c>
       <c r="I63" t="s" s="6">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J63" t="s" s="6">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" ht="20.05" customHeight="1">
       <c r="A64" t="s" s="6">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B64" s="7">
         <v>10</v>
@@ -3962,15 +3959,15 @@
         <v>15</v>
       </c>
       <c r="I64" t="s" s="6">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J64" t="s" s="6">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" ht="20.05" customHeight="1">
       <c r="A65" t="s" s="6">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B65" s="7">
         <v>0</v>
@@ -3994,15 +3991,15 @@
         <v>18</v>
       </c>
       <c r="I65" t="s" s="6">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J65" t="s" s="6">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" ht="20.05" customHeight="1">
       <c r="A66" t="s" s="6">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B66" s="7">
         <v>0</v>
@@ -4026,15 +4023,15 @@
         <v>18</v>
       </c>
       <c r="I66" t="s" s="6">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J66" t="s" s="6">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" ht="20.05" customHeight="1">
       <c r="A67" t="s" s="6">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B67" s="7">
         <v>34</v>
@@ -4058,15 +4055,15 @@
         <v>11</v>
       </c>
       <c r="I67" t="s" s="6">
+        <v>161</v>
+      </c>
+      <c r="J67" t="s" s="6">
         <v>162</v>
-      </c>
-      <c r="J67" t="s" s="6">
-        <v>163</v>
       </c>
     </row>
     <row r="68" ht="20.05" customHeight="1">
       <c r="A68" t="s" s="6">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B68" s="7">
         <v>25</v>
@@ -4090,15 +4087,15 @@
         <v>11</v>
       </c>
       <c r="I68" t="s" s="6">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J68" t="s" s="6">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" ht="20.05" customHeight="1">
       <c r="A69" t="s" s="6">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B69" s="7">
         <v>10</v>
@@ -4122,15 +4119,15 @@
         <v>15</v>
       </c>
       <c r="I69" t="s" s="6">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J69" t="s" s="6">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" ht="20.05" customHeight="1">
       <c r="A70" t="s" s="6">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B70" s="7">
         <v>7</v>
@@ -4154,15 +4151,15 @@
         <v>32</v>
       </c>
       <c r="I70" t="s" s="6">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J70" t="s" s="6">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" ht="20.05" customHeight="1">
       <c r="A71" t="s" s="6">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B71" s="7">
         <v>10</v>
@@ -4186,15 +4183,15 @@
         <v>18</v>
       </c>
       <c r="I71" t="s" s="6">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J71" t="s" s="6">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" ht="20.05" customHeight="1">
       <c r="A72" t="s" s="6">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B72" s="7">
         <v>0</v>
@@ -4218,15 +4215,15 @@
         <v>18</v>
       </c>
       <c r="I72" t="s" s="6">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J72" t="s" s="6">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" ht="20.05" customHeight="1">
       <c r="A73" t="s" s="6">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B73" s="7">
         <v>20</v>
@@ -4250,15 +4247,15 @@
         <v>11</v>
       </c>
       <c r="I73" t="s" s="6">
+        <v>174</v>
+      </c>
+      <c r="J73" t="s" s="6">
         <v>175</v>
-      </c>
-      <c r="J73" t="s" s="6">
-        <v>176</v>
       </c>
     </row>
     <row r="74" ht="20.05" customHeight="1">
       <c r="A74" t="s" s="6">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B74" s="7">
         <v>6</v>
@@ -4282,15 +4279,15 @@
         <v>15</v>
       </c>
       <c r="I74" t="s" s="6">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J74" t="s" s="6">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" ht="20.05" customHeight="1">
       <c r="A75" t="s" s="6">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B75" s="7">
         <v>0</v>
@@ -4314,15 +4311,15 @@
         <v>32</v>
       </c>
       <c r="I75" t="s" s="6">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J75" t="s" s="6">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" ht="20.05" customHeight="1">
       <c r="A76" t="s" s="6">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B76" s="7">
         <v>2</v>
@@ -4346,15 +4343,15 @@
         <v>18</v>
       </c>
       <c r="I76" t="s" s="6">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J76" t="s" s="6">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" ht="20.05" customHeight="1">
       <c r="A77" t="s" s="6">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B77" s="7">
         <v>13</v>
@@ -4378,15 +4375,15 @@
         <v>11</v>
       </c>
       <c r="I77" t="s" s="6">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J77" t="s" s="6">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" ht="20.05" customHeight="1">
       <c r="A78" t="s" s="6">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B78" s="7">
         <v>15</v>
@@ -4410,15 +4407,15 @@
         <v>11</v>
       </c>
       <c r="I78" t="s" s="6">
+        <v>185</v>
+      </c>
+      <c r="J78" t="s" s="6">
         <v>186</v>
-      </c>
-      <c r="J78" t="s" s="6">
-        <v>187</v>
       </c>
     </row>
     <row r="79" ht="20.05" customHeight="1">
       <c r="A79" t="s" s="6">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B79" s="7">
         <v>17</v>
@@ -4442,15 +4439,15 @@
         <v>11</v>
       </c>
       <c r="I79" t="s" s="6">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J79" t="s" s="6">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="80" ht="20.05" customHeight="1">
       <c r="A80" t="s" s="6">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B80" s="7">
         <v>10</v>
@@ -4474,15 +4471,15 @@
         <v>15</v>
       </c>
       <c r="I80" t="s" s="6">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J80" t="s" s="6">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="81" ht="20.05" customHeight="1">
       <c r="A81" t="s" s="6">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B81" s="7">
         <v>9</v>
@@ -4506,15 +4503,15 @@
         <v>15</v>
       </c>
       <c r="I81" t="s" s="6">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J81" t="s" s="6">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" ht="20.05" customHeight="1">
       <c r="A82" t="s" s="6">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B82" s="7">
         <v>1</v>
@@ -4538,15 +4535,15 @@
         <v>18</v>
       </c>
       <c r="I82" t="s" s="6">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J82" t="s" s="6">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" ht="20.05" customHeight="1">
       <c r="A83" t="s" s="6">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B83" s="7">
         <v>43</v>
@@ -4570,15 +4567,15 @@
         <v>11</v>
       </c>
       <c r="I83" t="s" s="6">
+        <v>196</v>
+      </c>
+      <c r="J83" t="s" s="6">
         <v>197</v>
-      </c>
-      <c r="J83" t="s" s="6">
-        <v>198</v>
       </c>
     </row>
     <row r="84" ht="20.05" customHeight="1">
       <c r="A84" t="s" s="6">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B84" s="7">
         <v>12</v>
@@ -4602,15 +4599,15 @@
         <v>15</v>
       </c>
       <c r="I84" t="s" s="6">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J84" t="s" s="6">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" ht="20.05" customHeight="1">
       <c r="A85" t="s" s="6">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B85" s="7">
         <v>26</v>
@@ -4634,15 +4631,15 @@
         <v>11</v>
       </c>
       <c r="I85" t="s" s="6">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J85" t="s" s="6">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" ht="20.05" customHeight="1">
       <c r="A86" t="s" s="6">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B86" s="7">
         <v>14</v>
@@ -4666,15 +4663,15 @@
         <v>15</v>
       </c>
       <c r="I86" t="s" s="6">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J86" t="s" s="6">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="87" ht="32.05" customHeight="1">
       <c r="A87" t="s" s="6">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B87" s="7">
         <v>2</v>
@@ -4695,18 +4692,18 @@
         <v>39</v>
       </c>
       <c r="H87" t="s" s="6">
+        <v>205</v>
+      </c>
+      <c r="I87" t="s" s="6">
+        <v>196</v>
+      </c>
+      <c r="J87" t="s" s="6">
         <v>206</v>
-      </c>
-      <c r="I87" t="s" s="6">
-        <v>197</v>
-      </c>
-      <c r="J87" t="s" s="6">
-        <v>207</v>
       </c>
     </row>
     <row r="88" ht="20.05" customHeight="1">
       <c r="A88" t="s" s="6">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B88" s="7">
         <v>1</v>
@@ -4730,15 +4727,15 @@
         <v>18</v>
       </c>
       <c r="I88" t="s" s="6">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J88" t="s" s="6">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" ht="20.05" customHeight="1">
       <c r="A89" t="s" s="6">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B89" s="7">
         <v>31</v>
@@ -4762,15 +4759,15 @@
         <v>11</v>
       </c>
       <c r="I89" t="s" s="6">
+        <v>210</v>
+      </c>
+      <c r="J89" t="s" s="6">
         <v>211</v>
-      </c>
-      <c r="J89" t="s" s="6">
-        <v>212</v>
       </c>
     </row>
     <row r="90" ht="20.05" customHeight="1">
       <c r="A90" t="s" s="6">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B90" s="7">
         <v>10</v>
@@ -4794,15 +4791,15 @@
         <v>11</v>
       </c>
       <c r="I90" t="s" s="6">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J90" t="s" s="6">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" ht="20.05" customHeight="1">
       <c r="A91" t="s" s="6">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B91" s="7">
         <v>15</v>
@@ -4826,15 +4823,15 @@
         <v>15</v>
       </c>
       <c r="I91" t="s" s="6">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J91" t="s" s="6">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" ht="20.05" customHeight="1">
       <c r="A92" t="s" s="6">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B92" s="7">
         <v>10</v>
@@ -4858,15 +4855,15 @@
         <v>32</v>
       </c>
       <c r="I92" t="s" s="6">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J92" t="s" s="6">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" ht="20.05" customHeight="1">
       <c r="A93" t="s" s="6">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B93" s="7">
         <v>1</v>
@@ -4890,15 +4887,15 @@
         <v>18</v>
       </c>
       <c r="I93" t="s" s="6">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J93" t="s" s="6">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="94" ht="32.05" customHeight="1">
       <c r="A94" t="s" s="6">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B94" s="7">
         <v>0</v>
@@ -4922,15 +4919,15 @@
         <v>18</v>
       </c>
       <c r="I94" t="s" s="6">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J94" t="s" s="6">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="95" ht="20.05" customHeight="1">
       <c r="A95" t="s" s="6">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B95" s="7">
         <v>10</v>
@@ -4954,15 +4951,15 @@
         <v>15</v>
       </c>
       <c r="I95" t="s" s="6">
+        <v>223</v>
+      </c>
+      <c r="J95" t="s" s="6">
         <v>224</v>
-      </c>
-      <c r="J95" t="s" s="6">
-        <v>225</v>
       </c>
     </row>
     <row r="96" ht="20.05" customHeight="1">
       <c r="A96" t="s" s="6">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B96" s="7">
         <v>20</v>
@@ -4986,15 +4983,15 @@
         <v>11</v>
       </c>
       <c r="I96" t="s" s="6">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J96" t="s" s="6">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="97" ht="20.05" customHeight="1">
       <c r="A97" t="s" s="6">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B97" s="7">
         <v>12</v>
@@ -5018,15 +5015,15 @@
         <v>15</v>
       </c>
       <c r="I97" t="s" s="6">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J97" t="s" s="6">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="98" ht="20.05" customHeight="1">
       <c r="A98" t="s" s="6">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B98" s="7">
         <v>6</v>
@@ -5050,15 +5047,15 @@
         <v>32</v>
       </c>
       <c r="I98" t="s" s="6">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J98" t="s" s="6">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" ht="20.05" customHeight="1">
       <c r="A99" t="s" s="6">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B99" s="7">
         <v>12</v>
@@ -5082,15 +5079,15 @@
         <v>15</v>
       </c>
       <c r="I99" t="s" s="6">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J99" t="s" s="6">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="100" ht="20.05" customHeight="1">
       <c r="A100" t="s" s="6">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B100" s="7">
         <v>0</v>
@@ -5114,10 +5111,10 @@
         <v>18</v>
       </c>
       <c r="I100" t="s" s="6">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J100" t="s" s="6">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add coach information to every team.
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -4043,7 +4043,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="7">
         <v>27</v>
@@ -4075,7 +4075,7 @@
         <v>2</v>
       </c>
       <c r="E68" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F68" s="7">
         <v>27</v>
@@ -4203,7 +4203,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" s="7">
         <v>7</v>

</xml_diff>

<commit_message>
Finish the playerlist by adding 2 players to their old team and done add all the players whose teams are whether qualify or not qualify.
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="347">
   <si>
     <t>id</t>
   </si>
@@ -103,6 +103,15 @@
     <t>cote_8</t>
   </si>
   <si>
+    <t>cote_1_AFC_2024</t>
+  </si>
+  <si>
+    <t>Ken Sudo</t>
+  </si>
+  <si>
+    <t>efc_1</t>
+  </si>
+  <si>
     <t>aot_10_AFC_2024</t>
   </si>
   <si>
@@ -154,13 +163,22 @@
     <t>aot_3</t>
   </si>
   <si>
+    <t>boboiboy_7_AFC_2024</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>boboiboy</t>
+  </si>
+  <si>
+    <t>efc_9</t>
+  </si>
+  <si>
     <t>boboiboy_8_AFC_2024</t>
   </si>
   <si>
     <t>Fang</t>
-  </si>
-  <si>
-    <t>boboiboy</t>
   </si>
   <si>
     <t>boboiboy_8</t>
@@ -1146,7 +1164,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1176,6 +1194,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2226,7 +2253,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:M145"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
@@ -2454,31 +2481,31 @@
         <v>31</v>
       </c>
       <c r="C6" s="8">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D6" s="8">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E6" s="8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F6" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" s="8">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H6" s="8">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I6" t="s" s="7">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s" s="7">
         <v>32</v>
-      </c>
-      <c r="K6" t="s" s="7">
-        <v>33</v>
       </c>
       <c r="L6" t="s" s="7">
         <v>18</v>
@@ -2489,19 +2516,19 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="B7" t="s" s="7">
-        <v>35</v>
-      </c>
       <c r="C7" s="8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="8">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E7" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="8">
         <v>0</v>
@@ -2513,10 +2540,10 @@
         <v>71</v>
       </c>
       <c r="I7" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K7" t="s" s="7">
         <v>36</v>
@@ -2536,13 +2563,13 @@
         <v>38</v>
       </c>
       <c r="C8" s="8">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D8" s="8">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E8" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="8">
         <v>0</v>
@@ -2557,7 +2584,7 @@
         <v>21</v>
       </c>
       <c r="J8" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K8" t="s" s="7">
         <v>39</v>
@@ -2577,13 +2604,13 @@
         <v>41</v>
       </c>
       <c r="C9" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="8">
         <v>0</v>
@@ -2595,10 +2622,10 @@
         <v>71</v>
       </c>
       <c r="I9" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K9" t="s" s="7">
         <v>42</v>
@@ -2618,10 +2645,10 @@
         <v>44</v>
       </c>
       <c r="C10" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" s="8">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E10" s="8">
         <v>0</v>
@@ -2636,33 +2663,33 @@
         <v>71</v>
       </c>
       <c r="I10" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="K10" t="s" s="7">
         <v>45</v>
       </c>
-      <c r="J10" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="K10" t="s" s="7">
+      <c r="L10" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="M10" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" t="s" s="7">
         <v>46</v>
       </c>
-      <c r="L10" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="M10" s="9">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="11" ht="32.05" customHeight="1">
-      <c r="A11" t="s" s="7">
+      <c r="B11" t="s" s="7">
         <v>47</v>
       </c>
-      <c r="B11" t="s" s="7">
-        <v>48</v>
-      </c>
       <c r="C11" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D11" s="8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
@@ -2674,16 +2701,16 @@
         <v>34</v>
       </c>
       <c r="H11" s="8">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s" s="7">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="K11" t="s" s="7">
         <v>49</v>
-      </c>
-      <c r="K11" t="s" s="7">
-        <v>50</v>
       </c>
       <c r="L11" t="s" s="7">
         <v>18</v>
@@ -2694,16 +2721,16 @@
     </row>
     <row r="12" ht="32.05" customHeight="1">
       <c r="A12" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s" s="7">
         <v>51</v>
       </c>
-      <c r="B12" t="s" s="7">
-        <v>52</v>
-      </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D12" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -2712,16 +2739,16 @@
         <v>1</v>
       </c>
       <c r="G12" s="8">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H12" s="8">
         <v>102</v>
       </c>
       <c r="I12" t="s" s="7">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J12" t="s" s="7">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s" s="7">
         <v>53</v>
@@ -2741,10 +2768,10 @@
         <v>55</v>
       </c>
       <c r="C13" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="8">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
@@ -2759,10 +2786,10 @@
         <v>102</v>
       </c>
       <c r="I13" t="s" s="7">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J13" t="s" s="7">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K13" t="s" s="7">
         <v>56</v>
@@ -2785,28 +2812,28 @@
         <v>0</v>
       </c>
       <c r="D14" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
       </c>
       <c r="F14" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="8">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H14" s="8">
         <v>102</v>
       </c>
       <c r="I14" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s" s="7">
+        <v>52</v>
+      </c>
+      <c r="K14" t="s" s="7">
         <v>59</v>
-      </c>
-      <c r="J14" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="K14" t="s" s="7">
-        <v>60</v>
       </c>
       <c r="L14" t="s" s="7">
         <v>18</v>
@@ -2817,16 +2844,16 @@
     </row>
     <row r="15" ht="32.05" customHeight="1">
       <c r="A15" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s" s="7">
         <v>61</v>
       </c>
-      <c r="B15" t="s" s="7">
-        <v>62</v>
-      </c>
       <c r="C15" s="8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D15" s="8">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E15" s="8">
         <v>0</v>
@@ -2835,19 +2862,19 @@
         <v>0</v>
       </c>
       <c r="G15" s="8">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H15" s="8">
         <v>102</v>
       </c>
       <c r="I15" t="s" s="7">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="J15" t="s" s="7">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s" s="7">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L15" t="s" s="7">
         <v>18</v>
@@ -2858,37 +2885,37 @@
     </row>
     <row r="16" ht="32.05" customHeight="1">
       <c r="A16" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>16</v>
+      </c>
+      <c r="H16" s="8">
+        <v>102</v>
+      </c>
+      <c r="I16" t="s" s="7">
         <v>65</v>
       </c>
-      <c r="B16" t="s" s="7">
+      <c r="J16" t="s" s="7">
+        <v>52</v>
+      </c>
+      <c r="K16" t="s" s="7">
         <v>66</v>
-      </c>
-      <c r="C16" s="8">
-        <v>22</v>
-      </c>
-      <c r="D16" s="8">
-        <v>26</v>
-      </c>
-      <c r="E16" s="8">
-        <v>1</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>34</v>
-      </c>
-      <c r="H16" s="8">
-        <v>41</v>
-      </c>
-      <c r="I16" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="J16" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="K16" t="s" s="7">
-        <v>68</v>
       </c>
       <c r="L16" t="s" s="7">
         <v>18</v>
@@ -2899,37 +2926,37 @@
     </row>
     <row r="17" ht="32.05" customHeight="1">
       <c r="A17" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s" s="7">
+        <v>68</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>23</v>
+      </c>
+      <c r="H17" s="8">
+        <v>102</v>
+      </c>
+      <c r="I17" t="s" s="7">
         <v>69</v>
       </c>
-      <c r="B17" t="s" s="7">
+      <c r="J17" t="s" s="7">
+        <v>52</v>
+      </c>
+      <c r="K17" t="s" s="7">
         <v>70</v>
-      </c>
-      <c r="C17" s="8">
-        <v>0</v>
-      </c>
-      <c r="D17" s="8">
-        <v>2</v>
-      </c>
-      <c r="E17" s="8">
-        <v>0</v>
-      </c>
-      <c r="F17" s="8">
-        <v>0</v>
-      </c>
-      <c r="G17" s="8">
-        <v>10</v>
-      </c>
-      <c r="H17" s="8">
-        <v>41</v>
-      </c>
-      <c r="I17" t="s" s="7">
-        <v>25</v>
-      </c>
-      <c r="J17" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="K17" t="s" s="7">
-        <v>71</v>
       </c>
       <c r="L17" t="s" s="7">
         <v>18</v>
@@ -2940,34 +2967,34 @@
     </row>
     <row r="18" ht="32.05" customHeight="1">
       <c r="A18" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s" s="7">
         <v>72</v>
       </c>
-      <c r="B18" t="s" s="7">
-        <v>73</v>
-      </c>
       <c r="C18" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D18" s="8">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="E18" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="8">
         <v>0</v>
       </c>
       <c r="G18" s="8">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H18" s="8">
         <v>41</v>
       </c>
       <c r="I18" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J18" t="s" s="7">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="K18" t="s" s="7">
         <v>74</v>
@@ -2987,7 +3014,7 @@
         <v>76</v>
       </c>
       <c r="C19" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D19" s="8">
         <v>2</v>
@@ -2999,16 +3026,16 @@
         <v>0</v>
       </c>
       <c r="G19" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H19" s="8">
         <v>41</v>
       </c>
       <c r="I19" t="s" s="7">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J19" t="s" s="7">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="K19" t="s" s="7">
         <v>77</v>
@@ -3028,7 +3055,7 @@
         <v>79</v>
       </c>
       <c r="C20" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20" s="8">
         <v>4</v>
@@ -3040,16 +3067,16 @@
         <v>0</v>
       </c>
       <c r="G20" s="8">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H20" s="8">
         <v>41</v>
       </c>
       <c r="I20" t="s" s="7">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J20" t="s" s="7">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="K20" t="s" s="7">
         <v>80</v>
@@ -3069,28 +3096,28 @@
         <v>82</v>
       </c>
       <c r="C21" s="8">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D21" s="8">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="E21" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="8">
         <v>0</v>
       </c>
       <c r="G21" s="8">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="H21" s="8">
         <v>41</v>
       </c>
       <c r="I21" t="s" s="7">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J21" t="s" s="7">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="K21" t="s" s="7">
         <v>83</v>
@@ -3110,28 +3137,28 @@
         <v>85</v>
       </c>
       <c r="C22" s="8">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="D22" s="8">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E22" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="8">
         <v>0</v>
       </c>
       <c r="G22" s="8">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="H22" s="8">
         <v>41</v>
       </c>
       <c r="I22" t="s" s="7">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J22" t="s" s="7">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="K22" t="s" s="7">
         <v>86</v>
@@ -3151,13 +3178,13 @@
         <v>88</v>
       </c>
       <c r="C23" s="8">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D23" s="8">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E23" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F23" s="8">
         <v>0</v>
@@ -3166,16 +3193,16 @@
         <v>34</v>
       </c>
       <c r="H23" s="8">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="I23" t="s" s="7">
         <v>15</v>
       </c>
       <c r="J23" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="K23" t="s" s="7">
         <v>89</v>
-      </c>
-      <c r="K23" t="s" s="7">
-        <v>90</v>
       </c>
       <c r="L23" t="s" s="7">
         <v>18</v>
@@ -3186,19 +3213,19 @@
     </row>
     <row r="24" ht="32.05" customHeight="1">
       <c r="A24" t="s" s="7">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s" s="7">
         <v>91</v>
       </c>
-      <c r="B24" t="s" s="7">
-        <v>92</v>
-      </c>
       <c r="C24" s="8">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D24" s="8">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E24" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" s="8">
         <v>0</v>
@@ -3207,16 +3234,16 @@
         <v>34</v>
       </c>
       <c r="H24" s="8">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="I24" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J24" t="s" s="7">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="K24" t="s" s="7">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L24" t="s" s="7">
         <v>18</v>
@@ -3227,19 +3254,19 @@
     </row>
     <row r="25" ht="32.05" customHeight="1">
       <c r="A25" t="s" s="7">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s" s="7">
         <v>94</v>
       </c>
-      <c r="B25" t="s" s="7">
-        <v>95</v>
-      </c>
       <c r="C25" s="8">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D25" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F25" s="8">
         <v>0</v>
@@ -3251,10 +3278,10 @@
         <v>60</v>
       </c>
       <c r="I25" t="s" s="7">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J25" t="s" s="7">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="K25" t="s" s="7">
         <v>96</v>
@@ -3274,13 +3301,13 @@
         <v>98</v>
       </c>
       <c r="C26" s="8">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D26" s="8">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E26" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" s="8">
         <v>0</v>
@@ -3295,7 +3322,7 @@
         <v>21</v>
       </c>
       <c r="J26" t="s" s="7">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="K26" t="s" s="7">
         <v>99</v>
@@ -3315,13 +3342,13 @@
         <v>101</v>
       </c>
       <c r="C27" s="8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D27" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E27" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" s="8">
         <v>0</v>
@@ -3333,10 +3360,10 @@
         <v>60</v>
       </c>
       <c r="I27" t="s" s="7">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="J27" t="s" s="7">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="K27" t="s" s="7">
         <v>102</v>
@@ -3348,7 +3375,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="28" ht="20.05" customHeight="1">
+    <row r="28" ht="32.05" customHeight="1">
       <c r="A28" t="s" s="7">
         <v>103</v>
       </c>
@@ -3359,10 +3386,10 @@
         <v>11</v>
       </c>
       <c r="D28" s="8">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E28" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="8">
         <v>0</v>
@@ -3371,39 +3398,39 @@
         <v>34</v>
       </c>
       <c r="H28" s="8">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="I28" t="s" s="7">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J28" t="s" s="7">
+        <v>95</v>
+      </c>
+      <c r="K28" t="s" s="7">
         <v>105</v>
       </c>
-      <c r="K28" t="s" s="7">
+      <c r="L28" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="M28" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="29" ht="32.05" customHeight="1">
+      <c r="A29" t="s" s="7">
         <v>106</v>
       </c>
-      <c r="L28" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="M28" s="9">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="7">
+      <c r="B29" t="s" s="7">
         <v>107</v>
       </c>
-      <c r="B29" t="s" s="7">
-        <v>108</v>
-      </c>
       <c r="C29" s="8">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D29" s="8">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E29" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F29" s="8">
         <v>0</v>
@@ -3412,16 +3439,16 @@
         <v>34</v>
       </c>
       <c r="H29" s="8">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="I29" t="s" s="7">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="J29" t="s" s="7">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="K29" t="s" s="7">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L29" t="s" s="7">
         <v>18</v>
@@ -3432,16 +3459,16 @@
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="7">
+        <v>109</v>
+      </c>
+      <c r="B30" t="s" s="7">
         <v>110</v>
       </c>
-      <c r="B30" t="s" s="7">
-        <v>111</v>
-      </c>
       <c r="C30" s="8">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D30" s="8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E30" s="8">
         <v>0</v>
@@ -3456,10 +3483,10 @@
         <v>114</v>
       </c>
       <c r="I30" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J30" t="s" s="7">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K30" t="s" s="7">
         <v>112</v>
@@ -3471,7 +3498,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="31" ht="32.05" customHeight="1">
+    <row r="31" ht="20.05" customHeight="1">
       <c r="A31" t="s" s="7">
         <v>113</v>
       </c>
@@ -3479,10 +3506,10 @@
         <v>114</v>
       </c>
       <c r="C31" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D31" s="8">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E31" s="8">
         <v>0</v>
@@ -3497,10 +3524,10 @@
         <v>114</v>
       </c>
       <c r="I31" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J31" t="s" s="7">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K31" t="s" s="7">
         <v>115</v>
@@ -3520,10 +3547,10 @@
         <v>117</v>
       </c>
       <c r="C32" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D32" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="8">
         <v>0</v>
@@ -3532,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="8">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H32" s="8">
         <v>114</v>
@@ -3541,7 +3568,7 @@
         <v>21</v>
       </c>
       <c r="J32" t="s" s="7">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K32" t="s" s="7">
         <v>118</v>
@@ -3553,7 +3580,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="33" ht="20.05" customHeight="1">
+    <row r="33" ht="32.05" customHeight="1">
       <c r="A33" t="s" s="7">
         <v>119</v>
       </c>
@@ -3561,10 +3588,10 @@
         <v>120</v>
       </c>
       <c r="C33" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E33" s="8">
         <v>0</v>
@@ -3579,10 +3606,10 @@
         <v>114</v>
       </c>
       <c r="I33" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J33" t="s" s="7">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K33" t="s" s="7">
         <v>121</v>
@@ -3602,31 +3629,31 @@
         <v>123</v>
       </c>
       <c r="C34" s="8">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D34" s="8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E34" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="8">
         <v>0</v>
       </c>
       <c r="G34" s="8">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="H34" s="8">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="I34" t="s" s="7">
         <v>21</v>
       </c>
       <c r="J34" t="s" s="7">
+        <v>111</v>
+      </c>
+      <c r="K34" t="s" s="7">
         <v>124</v>
-      </c>
-      <c r="K34" t="s" s="7">
-        <v>125</v>
       </c>
       <c r="L34" t="s" s="7">
         <v>18</v>
@@ -3637,19 +3664,19 @@
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" t="s" s="7">
+        <v>125</v>
+      </c>
+      <c r="B35" t="s" s="7">
         <v>126</v>
       </c>
-      <c r="B35" t="s" s="7">
-        <v>127</v>
-      </c>
       <c r="C35" s="8">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D35" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E35" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F35" s="8">
         <v>0</v>
@@ -3658,39 +3685,39 @@
         <v>34</v>
       </c>
       <c r="H35" s="8">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="I35" t="s" s="7">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J35" t="s" s="7">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="K35" t="s" s="7">
+        <v>127</v>
+      </c>
+      <c r="L35" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="M35" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" t="s" s="7">
         <v>128</v>
       </c>
-      <c r="L35" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="M35" s="9">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="36" ht="32.05" customHeight="1">
-      <c r="A36" t="s" s="7">
+      <c r="B36" t="s" s="7">
         <v>129</v>
       </c>
-      <c r="B36" t="s" s="7">
-        <v>130</v>
-      </c>
       <c r="C36" s="8">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D36" s="8">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E36" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F36" s="8">
         <v>0</v>
@@ -3705,7 +3732,7 @@
         <v>21</v>
       </c>
       <c r="J36" t="s" s="7">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K36" t="s" s="7">
         <v>131</v>
@@ -3725,28 +3752,28 @@
         <v>133</v>
       </c>
       <c r="C37" s="8">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D37" s="8">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E37" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F37" s="8">
         <v>0</v>
       </c>
       <c r="G37" s="8">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H37" s="8">
         <v>81</v>
       </c>
       <c r="I37" t="s" s="7">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J37" t="s" s="7">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K37" t="s" s="7">
         <v>134</v>
@@ -3758,7 +3785,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="38" ht="20.05" customHeight="1">
+    <row r="38" ht="32.05" customHeight="1">
       <c r="A38" t="s" s="7">
         <v>135</v>
       </c>
@@ -3766,28 +3793,28 @@
         <v>136</v>
       </c>
       <c r="C38" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D38" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E38" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F38" s="8">
         <v>0</v>
       </c>
       <c r="G38" s="8">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H38" s="8">
         <v>81</v>
       </c>
       <c r="I38" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J38" t="s" s="7">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K38" t="s" s="7">
         <v>137</v>
@@ -3807,28 +3834,28 @@
         <v>139</v>
       </c>
       <c r="C39" s="8">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D39" s="8">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E39" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F39" s="8">
         <v>0</v>
       </c>
       <c r="G39" s="8">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H39" s="8">
         <v>81</v>
       </c>
       <c r="I39" t="s" s="7">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J39" t="s" s="7">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K39" t="s" s="7">
         <v>140</v>
@@ -3840,7 +3867,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="40" ht="32.05" customHeight="1">
+    <row r="40" ht="20.05" customHeight="1">
       <c r="A40" t="s" s="7">
         <v>141</v>
       </c>
@@ -3848,10 +3875,10 @@
         <v>142</v>
       </c>
       <c r="C40" s="8">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <v>2</v>
@@ -3860,60 +3887,60 @@
         <v>0</v>
       </c>
       <c r="G40" s="8">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H40" s="8">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="I40" t="s" s="7">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J40" t="s" s="7">
+        <v>130</v>
+      </c>
+      <c r="K40" t="s" s="7">
         <v>143</v>
       </c>
-      <c r="K40" t="s" s="7">
+      <c r="L40" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="M40" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" t="s" s="7">
         <v>144</v>
       </c>
-      <c r="L40" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="M40" s="9">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="41" ht="32.05" customHeight="1">
-      <c r="A41" t="s" s="7">
+      <c r="B41" t="s" s="7">
         <v>145</v>
       </c>
-      <c r="B41" t="s" s="7">
-        <v>146</v>
-      </c>
       <c r="C41" s="8">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D41" s="8">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E41" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F41" s="8">
         <v>0</v>
       </c>
       <c r="G41" s="8">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H41" s="8">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="I41" t="s" s="7">
         <v>15</v>
       </c>
       <c r="J41" t="s" s="7">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="K41" t="s" s="7">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L41" t="s" s="7">
         <v>18</v>
@@ -3924,37 +3951,37 @@
     </row>
     <row r="42" ht="32.05" customHeight="1">
       <c r="A42" t="s" s="7">
+        <v>147</v>
+      </c>
+      <c r="B42" t="s" s="7">
         <v>148</v>
       </c>
-      <c r="B42" t="s" s="7">
-        <v>149</v>
-      </c>
       <c r="C42" s="8">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D42" s="8">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E42" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" s="8">
         <v>0</v>
       </c>
       <c r="G42" s="8">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H42" s="8">
         <v>35</v>
       </c>
       <c r="I42" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="J42" t="s" s="7">
+        <v>149</v>
+      </c>
+      <c r="K42" t="s" s="7">
         <v>150</v>
-      </c>
-      <c r="J42" t="s" s="7">
-        <v>143</v>
-      </c>
-      <c r="K42" t="s" s="7">
-        <v>151</v>
       </c>
       <c r="L42" t="s" s="7">
         <v>18</v>
@@ -3965,16 +3992,16 @@
     </row>
     <row r="43" ht="32.05" customHeight="1">
       <c r="A43" t="s" s="7">
+        <v>151</v>
+      </c>
+      <c r="B43" t="s" s="7">
         <v>152</v>
       </c>
-      <c r="B43" t="s" s="7">
-        <v>153</v>
-      </c>
       <c r="C43" s="8">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D43" s="8">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E43" s="8">
         <v>2</v>
@@ -3983,19 +4010,19 @@
         <v>0</v>
       </c>
       <c r="G43" s="8">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H43" s="8">
         <v>35</v>
       </c>
       <c r="I43" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J43" t="s" s="7">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="K43" t="s" s="7">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L43" t="s" s="7">
         <v>18</v>
@@ -4006,19 +4033,19 @@
     </row>
     <row r="44" ht="32.05" customHeight="1">
       <c r="A44" t="s" s="7">
+        <v>154</v>
+      </c>
+      <c r="B44" t="s" s="7">
         <v>155</v>
       </c>
-      <c r="B44" t="s" s="7">
-        <v>156</v>
-      </c>
       <c r="C44" s="8">
+        <v>16</v>
+      </c>
+      <c r="D44" s="8">
+        <v>5</v>
+      </c>
+      <c r="E44" s="8">
         <v>1</v>
-      </c>
-      <c r="D44" s="8">
-        <v>24</v>
-      </c>
-      <c r="E44" s="8">
-        <v>4</v>
       </c>
       <c r="F44" s="8">
         <v>0</v>
@@ -4030,10 +4057,10 @@
         <v>35</v>
       </c>
       <c r="I44" t="s" s="7">
-        <v>25</v>
+        <v>156</v>
       </c>
       <c r="J44" t="s" s="7">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="K44" t="s" s="7">
         <v>157</v>
@@ -4045,7 +4072,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="45" ht="20.05" customHeight="1">
+    <row r="45" ht="32.05" customHeight="1">
       <c r="A45" t="s" s="7">
         <v>158</v>
       </c>
@@ -4053,10 +4080,10 @@
         <v>159</v>
       </c>
       <c r="C45" s="8">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D45" s="8">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E45" s="8">
         <v>2</v>
@@ -4065,60 +4092,60 @@
         <v>0</v>
       </c>
       <c r="G45" s="8">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H45" s="8">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I45" t="s" s="7">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J45" t="s" s="7">
+        <v>149</v>
+      </c>
+      <c r="K45" t="s" s="7">
         <v>160</v>
       </c>
-      <c r="K45" t="s" s="7">
+      <c r="L45" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="M45" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="46" ht="32.05" customHeight="1">
+      <c r="A46" t="s" s="7">
         <v>161</v>
       </c>
-      <c r="L45" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="M45" s="9">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" t="s" s="7">
+      <c r="B46" t="s" s="7">
         <v>162</v>
       </c>
-      <c r="B46" t="s" s="7">
+      <c r="C46" s="8">
+        <v>1</v>
+      </c>
+      <c r="D46" s="8">
+        <v>24</v>
+      </c>
+      <c r="E46" s="8">
+        <v>4</v>
+      </c>
+      <c r="F46" s="8">
+        <v>0</v>
+      </c>
+      <c r="G46" s="8">
+        <v>34</v>
+      </c>
+      <c r="H46" s="8">
+        <v>35</v>
+      </c>
+      <c r="I46" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J46" t="s" s="7">
+        <v>149</v>
+      </c>
+      <c r="K46" t="s" s="7">
         <v>163</v>
-      </c>
-      <c r="C46" s="8">
-        <v>25</v>
-      </c>
-      <c r="D46" s="8">
-        <v>23</v>
-      </c>
-      <c r="E46" s="8">
-        <v>2</v>
-      </c>
-      <c r="F46" s="8">
-        <v>0</v>
-      </c>
-      <c r="G46" s="8">
-        <v>27</v>
-      </c>
-      <c r="H46" s="8">
-        <v>37</v>
-      </c>
-      <c r="I46" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="J46" t="s" s="7">
-        <v>160</v>
-      </c>
-      <c r="K46" t="s" s="7">
-        <v>164</v>
       </c>
       <c r="L46" t="s" s="7">
         <v>18</v>
@@ -4129,34 +4156,34 @@
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B47" t="s" s="7">
         <v>165</v>
       </c>
-      <c r="B47" t="s" s="7">
-        <v>166</v>
-      </c>
       <c r="C47" s="8">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D47" s="8">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E47" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F47" s="8">
         <v>0</v>
       </c>
       <c r="G47" s="8">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H47" s="8">
         <v>37</v>
       </c>
       <c r="I47" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J47" t="s" s="7">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="K47" t="s" s="7">
         <v>167</v>
@@ -4176,28 +4203,28 @@
         <v>169</v>
       </c>
       <c r="C48" s="8">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D48" s="8">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E48" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F48" s="8">
         <v>0</v>
       </c>
       <c r="G48" s="8">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H48" s="8">
         <v>37</v>
       </c>
       <c r="I48" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J48" t="s" s="7">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="K48" t="s" s="7">
         <v>170</v>
@@ -4217,19 +4244,19 @@
         <v>172</v>
       </c>
       <c r="C49" s="8">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D49" s="8">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E49" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="8">
         <v>0</v>
       </c>
       <c r="G49" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H49" s="8">
         <v>37</v>
@@ -4238,7 +4265,7 @@
         <v>21</v>
       </c>
       <c r="J49" t="s" s="7">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="K49" t="s" s="7">
         <v>173</v>
@@ -4258,28 +4285,28 @@
         <v>175</v>
       </c>
       <c r="C50" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D50" s="8">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E50" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" s="8">
         <v>0</v>
       </c>
       <c r="G50" s="8">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H50" s="8">
         <v>37</v>
       </c>
       <c r="I50" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J50" t="s" s="7">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="K50" t="s" s="7">
         <v>176</v>
@@ -4299,31 +4326,31 @@
         <v>178</v>
       </c>
       <c r="C51" s="8">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D51" s="8">
+        <v>6</v>
+      </c>
+      <c r="E51" s="8">
+        <v>0</v>
+      </c>
+      <c r="F51" s="8">
+        <v>0</v>
+      </c>
+      <c r="G51" s="8">
+        <v>10</v>
+      </c>
+      <c r="H51" s="8">
+        <v>37</v>
+      </c>
+      <c r="I51" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="E51" s="8">
-        <v>1</v>
-      </c>
-      <c r="F51" s="8">
-        <v>0</v>
-      </c>
-      <c r="G51" s="8">
-        <v>34</v>
-      </c>
-      <c r="H51" s="8">
-        <v>41</v>
-      </c>
-      <c r="I51" t="s" s="7">
-        <v>15</v>
-      </c>
       <c r="J51" t="s" s="7">
+        <v>166</v>
+      </c>
+      <c r="K51" t="s" s="7">
         <v>179</v>
-      </c>
-      <c r="K51" t="s" s="7">
-        <v>180</v>
       </c>
       <c r="L51" t="s" s="7">
         <v>18</v>
@@ -4334,19 +4361,19 @@
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="7">
+        <v>180</v>
+      </c>
+      <c r="B52" t="s" s="7">
         <v>181</v>
       </c>
-      <c r="B52" t="s" s="7">
-        <v>182</v>
-      </c>
       <c r="C52" s="8">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D52" s="8">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E52" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F52" s="8">
         <v>0</v>
@@ -4355,16 +4382,16 @@
         <v>34</v>
       </c>
       <c r="H52" s="8">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I52" t="s" s="7">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J52" t="s" s="7">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="K52" t="s" s="7">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L52" t="s" s="7">
         <v>18</v>
@@ -4375,34 +4402,34 @@
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="7">
+        <v>183</v>
+      </c>
+      <c r="B53" t="s" s="7">
         <v>184</v>
       </c>
-      <c r="B53" t="s" s="7">
-        <v>185</v>
-      </c>
       <c r="C53" s="8">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D53" s="8">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E53" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="8">
         <v>0</v>
       </c>
       <c r="G53" s="8">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="H53" s="8">
         <v>41</v>
       </c>
       <c r="I53" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J53" t="s" s="7">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="K53" t="s" s="7">
         <v>186</v>
@@ -4422,28 +4449,28 @@
         <v>188</v>
       </c>
       <c r="C54" s="8">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D54" s="8">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E54" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" s="8">
         <v>0</v>
       </c>
       <c r="G54" s="8">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="H54" s="8">
         <v>41</v>
       </c>
       <c r="I54" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J54" t="s" s="7">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="K54" t="s" s="7">
         <v>189</v>
@@ -4463,10 +4490,10 @@
         <v>191</v>
       </c>
       <c r="C55" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D55" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E55" s="8">
         <v>0</v>
@@ -4475,7 +4502,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H55" s="8">
         <v>41</v>
@@ -4484,7 +4511,7 @@
         <v>21</v>
       </c>
       <c r="J55" t="s" s="7">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="K55" t="s" s="7">
         <v>192</v>
@@ -4504,28 +4531,28 @@
         <v>194</v>
       </c>
       <c r="C56" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D56" s="8">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E56" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="8">
         <v>0</v>
       </c>
       <c r="G56" s="8">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H56" s="8">
         <v>41</v>
       </c>
       <c r="I56" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J56" t="s" s="7">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="K56" t="s" s="7">
         <v>195</v>
@@ -4545,31 +4572,31 @@
         <v>197</v>
       </c>
       <c r="C57" s="8">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D57" s="8">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E57" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F57" s="8">
         <v>0</v>
       </c>
       <c r="G57" s="8">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="H57" s="8">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I57" t="s" s="7">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J57" t="s" s="7">
+        <v>185</v>
+      </c>
+      <c r="K57" t="s" s="7">
         <v>198</v>
-      </c>
-      <c r="K57" t="s" s="7">
-        <v>199</v>
       </c>
       <c r="L57" t="s" s="7">
         <v>18</v>
@@ -4580,19 +4607,19 @@
     </row>
     <row r="58" ht="20.05" customHeight="1">
       <c r="A58" t="s" s="7">
+        <v>199</v>
+      </c>
+      <c r="B58" t="s" s="7">
         <v>200</v>
       </c>
-      <c r="B58" t="s" s="7">
-        <v>201</v>
-      </c>
       <c r="C58" s="8">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D58" s="8">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E58" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F58" s="8">
         <v>0</v>
@@ -4601,16 +4628,16 @@
         <v>34</v>
       </c>
       <c r="H58" s="8">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I58" t="s" s="7">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J58" t="s" s="7">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="K58" t="s" s="7">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L58" t="s" s="7">
         <v>18</v>
@@ -4621,19 +4648,19 @@
     </row>
     <row r="59" ht="20.05" customHeight="1">
       <c r="A59" t="s" s="7">
+        <v>202</v>
+      </c>
+      <c r="B59" t="s" s="7">
         <v>203</v>
       </c>
-      <c r="B59" t="s" s="7">
-        <v>204</v>
-      </c>
       <c r="C59" s="8">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D59" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E59" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F59" s="8">
         <v>0</v>
@@ -4645,10 +4672,10 @@
         <v>44</v>
       </c>
       <c r="I59" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J59" t="s" s="7">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="K59" t="s" s="7">
         <v>205</v>
@@ -4668,13 +4695,13 @@
         <v>207</v>
       </c>
       <c r="C60" s="8">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D60" s="8">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E60" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F60" s="8">
         <v>0</v>
@@ -4686,10 +4713,10 @@
         <v>44</v>
       </c>
       <c r="I60" t="s" s="7">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J60" t="s" s="7">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="K60" t="s" s="7">
         <v>208</v>
@@ -4709,13 +4736,13 @@
         <v>210</v>
       </c>
       <c r="C61" s="8">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D61" s="8">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E61" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" s="8">
         <v>0</v>
@@ -4727,10 +4754,10 @@
         <v>44</v>
       </c>
       <c r="I61" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J61" t="s" s="7">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="K61" t="s" s="7">
         <v>211</v>
@@ -4750,10 +4777,10 @@
         <v>213</v>
       </c>
       <c r="C62" s="8">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D62" s="8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E62" s="8">
         <v>1</v>
@@ -4765,16 +4792,16 @@
         <v>34</v>
       </c>
       <c r="H62" s="8">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="I62" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="J62" t="s" s="7">
+        <v>204</v>
+      </c>
+      <c r="K62" t="s" s="7">
         <v>214</v>
-      </c>
-      <c r="J62" t="s" s="7">
-        <v>215</v>
-      </c>
-      <c r="K62" t="s" s="7">
-        <v>216</v>
       </c>
       <c r="L62" t="s" s="7">
         <v>18</v>
@@ -4785,19 +4812,19 @@
     </row>
     <row r="63" ht="20.05" customHeight="1">
       <c r="A63" t="s" s="7">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B63" t="s" s="7">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C63" s="8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D63" s="8">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E63" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F63" s="8">
         <v>0</v>
@@ -4806,16 +4833,16 @@
         <v>34</v>
       </c>
       <c r="H63" s="8">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="I63" t="s" s="7">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J63" t="s" s="7">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="K63" t="s" s="7">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L63" t="s" s="7">
         <v>18</v>
@@ -4826,16 +4853,16 @@
     </row>
     <row r="64" ht="20.05" customHeight="1">
       <c r="A64" t="s" s="7">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B64" t="s" s="7">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C64" s="8">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D64" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E64" s="8">
         <v>1</v>
@@ -4850,10 +4877,10 @@
         <v>64</v>
       </c>
       <c r="I64" t="s" s="7">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="J64" t="s" s="7">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="K64" t="s" s="7">
         <v>222</v>
@@ -4873,13 +4900,13 @@
         <v>224</v>
       </c>
       <c r="C65" s="8">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D65" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E65" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" s="8">
         <v>0</v>
@@ -4894,7 +4921,7 @@
         <v>21</v>
       </c>
       <c r="J65" t="s" s="7">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="K65" t="s" s="7">
         <v>225</v>
@@ -4914,28 +4941,28 @@
         <v>227</v>
       </c>
       <c r="C66" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D66" s="8">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E66" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" s="8">
         <v>0</v>
       </c>
       <c r="G66" s="8">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H66" s="8">
         <v>64</v>
       </c>
       <c r="I66" t="s" s="7">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J66" t="s" s="7">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="K66" t="s" s="7">
         <v>228</v>
@@ -4955,10 +4982,10 @@
         <v>230</v>
       </c>
       <c r="C67" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D67" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E67" s="8">
         <v>0</v>
@@ -4967,16 +4994,16 @@
         <v>0</v>
       </c>
       <c r="G67" s="8">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="H67" s="8">
         <v>64</v>
       </c>
       <c r="I67" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J67" t="s" s="7">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="K67" t="s" s="7">
         <v>231</v>
@@ -4996,31 +5023,31 @@
         <v>233</v>
       </c>
       <c r="C68" s="8">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D68" s="8">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E68" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="8">
         <v>0</v>
       </c>
       <c r="G68" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H68" s="8">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="I68" t="s" s="7">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J68" t="s" s="7">
+        <v>221</v>
+      </c>
+      <c r="K68" t="s" s="7">
         <v>234</v>
-      </c>
-      <c r="K68" t="s" s="7">
-        <v>235</v>
       </c>
       <c r="L68" t="s" s="7">
         <v>18</v>
@@ -5031,37 +5058,37 @@
     </row>
     <row r="69" ht="20.05" customHeight="1">
       <c r="A69" t="s" s="7">
+        <v>235</v>
+      </c>
+      <c r="B69" t="s" s="7">
         <v>236</v>
       </c>
-      <c r="B69" t="s" s="7">
+      <c r="C69" s="8">
+        <v>0</v>
+      </c>
+      <c r="D69" s="8">
+        <v>0</v>
+      </c>
+      <c r="E69" s="8">
+        <v>0</v>
+      </c>
+      <c r="F69" s="8">
+        <v>0</v>
+      </c>
+      <c r="G69" s="8">
+        <v>5</v>
+      </c>
+      <c r="H69" s="8">
+        <v>64</v>
+      </c>
+      <c r="I69" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J69" t="s" s="7">
+        <v>221</v>
+      </c>
+      <c r="K69" t="s" s="7">
         <v>237</v>
-      </c>
-      <c r="C69" s="8">
-        <v>25</v>
-      </c>
-      <c r="D69" s="8">
-        <v>17</v>
-      </c>
-      <c r="E69" s="8">
-        <v>2</v>
-      </c>
-      <c r="F69" s="8">
-        <v>0</v>
-      </c>
-      <c r="G69" s="8">
-        <v>27</v>
-      </c>
-      <c r="H69" s="8">
-        <v>42</v>
-      </c>
-      <c r="I69" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="J69" t="s" s="7">
-        <v>234</v>
-      </c>
-      <c r="K69" t="s" s="7">
-        <v>238</v>
       </c>
       <c r="L69" t="s" s="7">
         <v>18</v>
@@ -5072,34 +5099,34 @@
     </row>
     <row r="70" ht="20.05" customHeight="1">
       <c r="A70" t="s" s="7">
+        <v>238</v>
+      </c>
+      <c r="B70" t="s" s="7">
         <v>239</v>
       </c>
-      <c r="B70" t="s" s="7">
-        <v>240</v>
-      </c>
       <c r="C70" s="8">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D70" s="8">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E70" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" s="8">
         <v>0</v>
       </c>
       <c r="G70" s="8">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H70" s="8">
         <v>42</v>
       </c>
       <c r="I70" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J70" t="s" s="7">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="K70" t="s" s="7">
         <v>241</v>
@@ -5119,28 +5146,28 @@
         <v>243</v>
       </c>
       <c r="C71" s="8">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D71" s="8">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E71" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F71" s="8">
         <v>0</v>
       </c>
       <c r="G71" s="8">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H71" s="8">
         <v>42</v>
       </c>
       <c r="I71" t="s" s="7">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J71" t="s" s="7">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="K71" t="s" s="7">
         <v>244</v>
@@ -5163,7 +5190,7 @@
         <v>10</v>
       </c>
       <c r="D72" s="8">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E72" s="8">
         <v>0</v>
@@ -5172,16 +5199,16 @@
         <v>0</v>
       </c>
       <c r="G72" s="8">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H72" s="8">
         <v>42</v>
       </c>
       <c r="I72" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J72" t="s" s="7">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="K72" t="s" s="7">
         <v>247</v>
@@ -5201,28 +5228,28 @@
         <v>249</v>
       </c>
       <c r="C73" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D73" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E73" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" s="8">
         <v>0</v>
       </c>
       <c r="G73" s="8">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H73" s="8">
         <v>42</v>
       </c>
       <c r="I73" t="s" s="7">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="J73" t="s" s="7">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="K73" t="s" s="7">
         <v>250</v>
@@ -5242,10 +5269,10 @@
         <v>252</v>
       </c>
       <c r="C74" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D74" s="8">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E74" s="8">
         <v>0</v>
@@ -5254,19 +5281,19 @@
         <v>0</v>
       </c>
       <c r="G74" s="8">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H74" s="8">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="I74" t="s" s="7">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J74" t="s" s="7">
+        <v>240</v>
+      </c>
+      <c r="K74" t="s" s="7">
         <v>253</v>
-      </c>
-      <c r="K74" t="s" s="7">
-        <v>254</v>
       </c>
       <c r="L74" t="s" s="7">
         <v>18</v>
@@ -5277,37 +5304,37 @@
     </row>
     <row r="75" ht="20.05" customHeight="1">
       <c r="A75" t="s" s="7">
+        <v>254</v>
+      </c>
+      <c r="B75" t="s" s="7">
         <v>255</v>
       </c>
-      <c r="B75" t="s" s="7">
+      <c r="C75" s="8">
+        <v>0</v>
+      </c>
+      <c r="D75" s="8">
+        <v>4</v>
+      </c>
+      <c r="E75" s="8">
+        <v>1</v>
+      </c>
+      <c r="F75" s="8">
+        <v>0</v>
+      </c>
+      <c r="G75" s="8">
+        <v>7</v>
+      </c>
+      <c r="H75" s="8">
+        <v>42</v>
+      </c>
+      <c r="I75" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J75" t="s" s="7">
+        <v>240</v>
+      </c>
+      <c r="K75" t="s" s="7">
         <v>256</v>
-      </c>
-      <c r="C75" s="8">
-        <v>6</v>
-      </c>
-      <c r="D75" s="8">
-        <v>8</v>
-      </c>
-      <c r="E75" s="8">
-        <v>0</v>
-      </c>
-      <c r="F75" s="8">
-        <v>0</v>
-      </c>
-      <c r="G75" s="8">
-        <v>34</v>
-      </c>
-      <c r="H75" s="8">
-        <v>75</v>
-      </c>
-      <c r="I75" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="J75" t="s" s="7">
-        <v>253</v>
-      </c>
-      <c r="K75" t="s" s="7">
-        <v>257</v>
       </c>
       <c r="L75" t="s" s="7">
         <v>18</v>
@@ -5318,16 +5345,16 @@
     </row>
     <row r="76" ht="20.05" customHeight="1">
       <c r="A76" t="s" s="7">
+        <v>257</v>
+      </c>
+      <c r="B76" t="s" s="7">
         <v>258</v>
       </c>
-      <c r="B76" t="s" s="7">
-        <v>259</v>
-      </c>
       <c r="C76" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D76" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E76" s="8">
         <v>0</v>
@@ -5342,10 +5369,10 @@
         <v>75</v>
       </c>
       <c r="I76" t="s" s="7">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J76" t="s" s="7">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="K76" t="s" s="7">
         <v>260</v>
@@ -5365,13 +5392,13 @@
         <v>262</v>
       </c>
       <c r="C77" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D77" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E77" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="8">
         <v>0</v>
@@ -5383,10 +5410,10 @@
         <v>75</v>
       </c>
       <c r="I77" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J77" t="s" s="7">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="K77" t="s" s="7">
         <v>263</v>
@@ -5406,10 +5433,10 @@
         <v>265</v>
       </c>
       <c r="C78" s="8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D78" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E78" s="8">
         <v>0</v>
@@ -5424,10 +5451,10 @@
         <v>75</v>
       </c>
       <c r="I78" t="s" s="7">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="J78" t="s" s="7">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="K78" t="s" s="7">
         <v>266</v>
@@ -5447,13 +5474,13 @@
         <v>268</v>
       </c>
       <c r="C79" s="8">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D79" s="8">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E79" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="8">
         <v>0</v>
@@ -5462,16 +5489,16 @@
         <v>34</v>
       </c>
       <c r="H79" s="8">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I79" t="s" s="7">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J79" t="s" s="7">
+        <v>259</v>
+      </c>
+      <c r="K79" t="s" s="7">
         <v>269</v>
-      </c>
-      <c r="K79" t="s" s="7">
-        <v>270</v>
       </c>
       <c r="L79" t="s" s="7">
         <v>18</v>
@@ -5482,13 +5509,13 @@
     </row>
     <row r="80" ht="20.05" customHeight="1">
       <c r="A80" t="s" s="7">
+        <v>270</v>
+      </c>
+      <c r="B80" t="s" s="7">
         <v>271</v>
       </c>
-      <c r="B80" t="s" s="7">
-        <v>272</v>
-      </c>
       <c r="C80" s="8">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D80" s="8">
         <v>10</v>
@@ -5497,22 +5524,22 @@
         <v>0</v>
       </c>
       <c r="F80" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G80" s="8">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H80" s="8">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I80" t="s" s="7">
         <v>15</v>
       </c>
       <c r="J80" t="s" s="7">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="K80" t="s" s="7">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L80" t="s" s="7">
         <v>18</v>
@@ -5523,16 +5550,16 @@
     </row>
     <row r="81" ht="20.05" customHeight="1">
       <c r="A81" t="s" s="7">
+        <v>273</v>
+      </c>
+      <c r="B81" t="s" s="7">
         <v>274</v>
       </c>
-      <c r="B81" t="s" s="7">
-        <v>275</v>
-      </c>
       <c r="C81" s="8">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D81" s="8">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E81" s="8">
         <v>0</v>
@@ -5547,10 +5574,10 @@
         <v>81</v>
       </c>
       <c r="I81" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J81" t="s" s="7">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="K81" t="s" s="7">
         <v>276</v>
@@ -5570,28 +5597,28 @@
         <v>278</v>
       </c>
       <c r="C82" s="8">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D82" s="8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E82" s="8">
         <v>0</v>
       </c>
       <c r="F82" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="8">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H82" s="8">
         <v>81</v>
       </c>
       <c r="I82" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J82" t="s" s="7">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="K82" t="s" s="7">
         <v>279</v>
@@ -5611,10 +5638,10 @@
         <v>281</v>
       </c>
       <c r="C83" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D83" s="8">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E83" s="8">
         <v>0</v>
@@ -5629,10 +5656,10 @@
         <v>81</v>
       </c>
       <c r="I83" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J83" t="s" s="7">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="K83" t="s" s="7">
         <v>282</v>
@@ -5652,7 +5679,7 @@
         <v>284</v>
       </c>
       <c r="C84" s="8">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="D84" s="8">
         <v>4</v>
@@ -5664,19 +5691,19 @@
         <v>0</v>
       </c>
       <c r="G84" s="8">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H84" s="8">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="I84" t="s" s="7">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J84" t="s" s="7">
+        <v>275</v>
+      </c>
+      <c r="K84" t="s" s="7">
         <v>285</v>
-      </c>
-      <c r="K84" t="s" s="7">
-        <v>286</v>
       </c>
       <c r="L84" t="s" s="7">
         <v>18</v>
@@ -5687,37 +5714,37 @@
     </row>
     <row r="85" ht="20.05" customHeight="1">
       <c r="A85" t="s" s="7">
+        <v>286</v>
+      </c>
+      <c r="B85" t="s" s="7">
         <v>287</v>
       </c>
-      <c r="B85" t="s" s="7">
+      <c r="C85" s="8">
+        <v>1</v>
+      </c>
+      <c r="D85" s="8">
+        <v>13</v>
+      </c>
+      <c r="E85" s="8">
+        <v>0</v>
+      </c>
+      <c r="F85" s="8">
+        <v>0</v>
+      </c>
+      <c r="G85" s="8">
+        <v>34</v>
+      </c>
+      <c r="H85" s="8">
+        <v>81</v>
+      </c>
+      <c r="I85" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J85" t="s" s="7">
+        <v>275</v>
+      </c>
+      <c r="K85" t="s" s="7">
         <v>288</v>
-      </c>
-      <c r="C85" s="8">
-        <v>12</v>
-      </c>
-      <c r="D85" s="8">
-        <v>44</v>
-      </c>
-      <c r="E85" s="8">
-        <v>0</v>
-      </c>
-      <c r="F85" s="8">
-        <v>0</v>
-      </c>
-      <c r="G85" s="8">
-        <v>29</v>
-      </c>
-      <c r="H85" s="8">
-        <v>39</v>
-      </c>
-      <c r="I85" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="J85" t="s" s="7">
-        <v>285</v>
-      </c>
-      <c r="K85" t="s" s="7">
-        <v>289</v>
       </c>
       <c r="L85" t="s" s="7">
         <v>18</v>
@@ -5728,16 +5755,16 @@
     </row>
     <row r="86" ht="20.05" customHeight="1">
       <c r="A86" t="s" s="7">
+        <v>289</v>
+      </c>
+      <c r="B86" t="s" s="7">
         <v>290</v>
       </c>
-      <c r="B86" t="s" s="7">
-        <v>291</v>
-      </c>
       <c r="C86" s="8">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D86" s="8">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E86" s="8">
         <v>0</v>
@@ -5746,7 +5773,7 @@
         <v>0</v>
       </c>
       <c r="G86" s="8">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H86" s="8">
         <v>39</v>
@@ -5755,7 +5782,7 @@
         <v>15</v>
       </c>
       <c r="J86" t="s" s="7">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="K86" t="s" s="7">
         <v>292</v>
@@ -5775,10 +5802,10 @@
         <v>294</v>
       </c>
       <c r="C87" s="8">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D87" s="8">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="E87" s="8">
         <v>0</v>
@@ -5787,7 +5814,7 @@
         <v>0</v>
       </c>
       <c r="G87" s="8">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H87" s="8">
         <v>39</v>
@@ -5796,7 +5823,7 @@
         <v>21</v>
       </c>
       <c r="J87" t="s" s="7">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="K87" t="s" s="7">
         <v>295</v>
@@ -5808,7 +5835,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="88" ht="32.05" customHeight="1">
+    <row r="88" ht="20.05" customHeight="1">
       <c r="A88" t="s" s="7">
         <v>296</v>
       </c>
@@ -5816,10 +5843,10 @@
         <v>297</v>
       </c>
       <c r="C88" s="8">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D88" s="8">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E88" s="8">
         <v>0</v>
@@ -5828,19 +5855,19 @@
         <v>0</v>
       </c>
       <c r="G88" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H88" s="8">
         <v>39</v>
       </c>
       <c r="I88" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="J88" t="s" s="7">
+        <v>291</v>
+      </c>
+      <c r="K88" t="s" s="7">
         <v>298</v>
-      </c>
-      <c r="J88" t="s" s="7">
-        <v>285</v>
-      </c>
-      <c r="K88" t="s" s="7">
-        <v>299</v>
       </c>
       <c r="L88" t="s" s="7">
         <v>18</v>
@@ -5851,16 +5878,16 @@
     </row>
     <row r="89" ht="20.05" customHeight="1">
       <c r="A89" t="s" s="7">
+        <v>299</v>
+      </c>
+      <c r="B89" t="s" s="7">
         <v>300</v>
       </c>
-      <c r="B89" t="s" s="7">
-        <v>301</v>
-      </c>
       <c r="C89" s="8">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D89" s="8">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E89" s="8">
         <v>0</v>
@@ -5869,60 +5896,60 @@
         <v>0</v>
       </c>
       <c r="G89" s="8">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="H89" s="8">
         <v>39</v>
       </c>
       <c r="I89" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J89" t="s" s="7">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="K89" t="s" s="7">
+        <v>301</v>
+      </c>
+      <c r="L89" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="M89" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="90" ht="32.05" customHeight="1">
+      <c r="A90" t="s" s="7">
         <v>302</v>
       </c>
-      <c r="L89" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="M89" s="9">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="90" ht="20.05" customHeight="1">
-      <c r="A90" t="s" s="7">
+      <c r="B90" t="s" s="7">
         <v>303</v>
       </c>
-      <c r="B90" t="s" s="7">
+      <c r="C90" s="8">
+        <v>2</v>
+      </c>
+      <c r="D90" s="8">
+        <v>15</v>
+      </c>
+      <c r="E90" s="8">
+        <v>0</v>
+      </c>
+      <c r="F90" s="8">
+        <v>0</v>
+      </c>
+      <c r="G90" s="8">
+        <v>27</v>
+      </c>
+      <c r="H90" s="8">
+        <v>39</v>
+      </c>
+      <c r="I90" t="s" s="7">
         <v>304</v>
       </c>
-      <c r="C90" s="8">
-        <v>31</v>
-      </c>
-      <c r="D90" s="8">
-        <v>22</v>
-      </c>
-      <c r="E90" s="8">
-        <v>0</v>
-      </c>
-      <c r="F90" s="8">
-        <v>0</v>
-      </c>
-      <c r="G90" s="8">
-        <v>34</v>
-      </c>
-      <c r="H90" s="8">
-        <v>61</v>
-      </c>
-      <c r="I90" t="s" s="7">
-        <v>15</v>
-      </c>
       <c r="J90" t="s" s="7">
+        <v>291</v>
+      </c>
+      <c r="K90" t="s" s="7">
         <v>305</v>
-      </c>
-      <c r="K90" t="s" s="7">
-        <v>306</v>
       </c>
       <c r="L90" t="s" s="7">
         <v>18</v>
@@ -5933,37 +5960,37 @@
     </row>
     <row r="91" ht="20.05" customHeight="1">
       <c r="A91" t="s" s="7">
+        <v>306</v>
+      </c>
+      <c r="B91" t="s" s="7">
         <v>307</v>
       </c>
-      <c r="B91" t="s" s="7">
+      <c r="C91" s="8">
+        <v>1</v>
+      </c>
+      <c r="D91" s="8">
+        <v>3</v>
+      </c>
+      <c r="E91" s="8">
+        <v>0</v>
+      </c>
+      <c r="F91" s="8">
+        <v>0</v>
+      </c>
+      <c r="G91" s="8">
+        <v>7</v>
+      </c>
+      <c r="H91" s="8">
+        <v>39</v>
+      </c>
+      <c r="I91" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J91" t="s" s="7">
+        <v>291</v>
+      </c>
+      <c r="K91" t="s" s="7">
         <v>308</v>
-      </c>
-      <c r="C91" s="8">
-        <v>10</v>
-      </c>
-      <c r="D91" s="8">
-        <v>6</v>
-      </c>
-      <c r="E91" s="8">
-        <v>0</v>
-      </c>
-      <c r="F91" s="8">
-        <v>0</v>
-      </c>
-      <c r="G91" s="8">
-        <v>34</v>
-      </c>
-      <c r="H91" s="8">
-        <v>61</v>
-      </c>
-      <c r="I91" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="J91" t="s" s="7">
-        <v>305</v>
-      </c>
-      <c r="K91" t="s" s="7">
-        <v>309</v>
       </c>
       <c r="L91" t="s" s="7">
         <v>18</v>
@@ -5974,16 +6001,16 @@
     </row>
     <row r="92" ht="20.05" customHeight="1">
       <c r="A92" t="s" s="7">
+        <v>309</v>
+      </c>
+      <c r="B92" t="s" s="7">
         <v>310</v>
       </c>
-      <c r="B92" t="s" s="7">
-        <v>311</v>
-      </c>
       <c r="C92" s="8">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D92" s="8">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E92" s="8">
         <v>0</v>
@@ -5998,10 +6025,10 @@
         <v>61</v>
       </c>
       <c r="I92" t="s" s="7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J92" t="s" s="7">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="K92" t="s" s="7">
         <v>312</v>
@@ -6024,7 +6051,7 @@
         <v>10</v>
       </c>
       <c r="D93" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E93" s="8">
         <v>0</v>
@@ -6039,10 +6066,10 @@
         <v>61</v>
       </c>
       <c r="I93" t="s" s="7">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J93" t="s" s="7">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="K93" t="s" s="7">
         <v>315</v>
@@ -6062,10 +6089,10 @@
         <v>317</v>
       </c>
       <c r="C94" s="8">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D94" s="8">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E94" s="8">
         <v>0</v>
@@ -6074,16 +6101,16 @@
         <v>0</v>
       </c>
       <c r="G94" s="8">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H94" s="8">
         <v>61</v>
       </c>
       <c r="I94" t="s" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J94" t="s" s="7">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="K94" t="s" s="7">
         <v>318</v>
@@ -6095,7 +6122,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="95" ht="32.05" customHeight="1">
+    <row r="95" ht="20.05" customHeight="1">
       <c r="A95" t="s" s="7">
         <v>319</v>
       </c>
@@ -6103,10 +6130,10 @@
         <v>320</v>
       </c>
       <c r="C95" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D95" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E95" s="8">
         <v>0</v>
@@ -6115,16 +6142,16 @@
         <v>0</v>
       </c>
       <c r="G95" s="8">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="H95" s="8">
         <v>61</v>
       </c>
       <c r="I95" t="s" s="7">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="J95" t="s" s="7">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="K95" t="s" s="7">
         <v>321</v>
@@ -6136,7 +6163,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="96" ht="32.05" customHeight="1">
+    <row r="96" ht="20.05" customHeight="1">
       <c r="A96" t="s" s="7">
         <v>322</v>
       </c>
@@ -6144,10 +6171,10 @@
         <v>323</v>
       </c>
       <c r="C96" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D96" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E96" s="8">
         <v>0</v>
@@ -6156,19 +6183,19 @@
         <v>0</v>
       </c>
       <c r="G96" s="8">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H96" s="8">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I96" t="s" s="7">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J96" t="s" s="7">
+        <v>311</v>
+      </c>
+      <c r="K96" t="s" s="7">
         <v>324</v>
-      </c>
-      <c r="K96" t="s" s="7">
-        <v>325</v>
       </c>
       <c r="L96" t="s" s="7">
         <v>18</v>
@@ -6179,37 +6206,37 @@
     </row>
     <row r="97" ht="32.05" customHeight="1">
       <c r="A97" t="s" s="7">
+        <v>325</v>
+      </c>
+      <c r="B97" t="s" s="7">
         <v>326</v>
       </c>
-      <c r="B97" t="s" s="7">
+      <c r="C97" s="8">
+        <v>0</v>
+      </c>
+      <c r="D97" s="8">
+        <v>2</v>
+      </c>
+      <c r="E97" s="8">
+        <v>0</v>
+      </c>
+      <c r="F97" s="8">
+        <v>0</v>
+      </c>
+      <c r="G97" s="8">
+        <v>15</v>
+      </c>
+      <c r="H97" s="8">
+        <v>61</v>
+      </c>
+      <c r="I97" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J97" t="s" s="7">
+        <v>311</v>
+      </c>
+      <c r="K97" t="s" s="7">
         <v>327</v>
-      </c>
-      <c r="C97" s="8">
-        <v>20</v>
-      </c>
-      <c r="D97" s="8">
-        <v>16</v>
-      </c>
-      <c r="E97" s="8">
-        <v>0</v>
-      </c>
-      <c r="F97" s="8">
-        <v>0</v>
-      </c>
-      <c r="G97" s="8">
-        <v>29</v>
-      </c>
-      <c r="H97" s="8">
-        <v>60</v>
-      </c>
-      <c r="I97" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="J97" t="s" s="7">
-        <v>324</v>
-      </c>
-      <c r="K97" t="s" s="7">
-        <v>328</v>
       </c>
       <c r="L97" t="s" s="7">
         <v>18</v>
@@ -6220,16 +6247,16 @@
     </row>
     <row r="98" ht="32.05" customHeight="1">
       <c r="A98" t="s" s="7">
+        <v>328</v>
+      </c>
+      <c r="B98" t="s" s="7">
         <v>329</v>
       </c>
-      <c r="B98" t="s" s="7">
-        <v>330</v>
-      </c>
       <c r="C98" s="8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D98" s="8">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E98" s="8">
         <v>0</v>
@@ -6238,7 +6265,7 @@
         <v>0</v>
       </c>
       <c r="G98" s="8">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H98" s="8">
         <v>60</v>
@@ -6247,7 +6274,7 @@
         <v>21</v>
       </c>
       <c r="J98" t="s" s="7">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="K98" t="s" s="7">
         <v>331</v>
@@ -6267,28 +6294,28 @@
         <v>333</v>
       </c>
       <c r="C99" s="8">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D99" s="8">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E99" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" s="8">
         <v>0</v>
       </c>
       <c r="G99" s="8">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H99" s="8">
         <v>60</v>
       </c>
       <c r="I99" t="s" s="7">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J99" t="s" s="7">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="K99" t="s" s="7">
         <v>334</v>
@@ -6311,7 +6338,7 @@
         <v>12</v>
       </c>
       <c r="D100" s="8">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E100" s="8">
         <v>0</v>
@@ -6320,7 +6347,7 @@
         <v>0</v>
       </c>
       <c r="G100" s="8">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H100" s="8">
         <v>60</v>
@@ -6329,7 +6356,7 @@
         <v>21</v>
       </c>
       <c r="J100" t="s" s="7">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="K100" t="s" s="7">
         <v>337</v>
@@ -6349,28 +6376,28 @@
         <v>339</v>
       </c>
       <c r="C101" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D101" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E101" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" s="8">
         <v>0</v>
       </c>
       <c r="G101" s="8">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="H101" s="8">
         <v>60</v>
       </c>
       <c r="I101" t="s" s="7">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="J101" t="s" s="7">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="K101" t="s" s="7">
         <v>340</v>
@@ -6381,6 +6408,718 @@
       <c r="M101" s="9">
         <v>2024</v>
       </c>
+    </row>
+    <row r="102" ht="32.05" customHeight="1">
+      <c r="A102" t="s" s="7">
+        <v>341</v>
+      </c>
+      <c r="B102" t="s" s="7">
+        <v>342</v>
+      </c>
+      <c r="C102" s="8">
+        <v>12</v>
+      </c>
+      <c r="D102" s="8">
+        <v>2</v>
+      </c>
+      <c r="E102" s="8">
+        <v>0</v>
+      </c>
+      <c r="F102" s="8">
+        <v>0</v>
+      </c>
+      <c r="G102" s="8">
+        <v>22</v>
+      </c>
+      <c r="H102" s="8">
+        <v>60</v>
+      </c>
+      <c r="I102" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="J102" t="s" s="7">
+        <v>330</v>
+      </c>
+      <c r="K102" t="s" s="7">
+        <v>343</v>
+      </c>
+      <c r="L102" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="M102" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="103" ht="32.05" customHeight="1">
+      <c r="A103" t="s" s="7">
+        <v>344</v>
+      </c>
+      <c r="B103" t="s" s="7">
+        <v>345</v>
+      </c>
+      <c r="C103" s="8">
+        <v>0</v>
+      </c>
+      <c r="D103" s="8">
+        <v>6</v>
+      </c>
+      <c r="E103" s="8">
+        <v>0</v>
+      </c>
+      <c r="F103" s="8">
+        <v>0</v>
+      </c>
+      <c r="G103" s="8">
+        <v>34</v>
+      </c>
+      <c r="H103" s="8">
+        <v>60</v>
+      </c>
+      <c r="I103" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J103" t="s" s="7">
+        <v>330</v>
+      </c>
+      <c r="K103" t="s" s="7">
+        <v>346</v>
+      </c>
+      <c r="L103" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="M103" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="104" ht="20.05" customHeight="1">
+      <c r="A104" s="10"/>
+      <c r="B104" s="10"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+      <c r="G104" s="10"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+      <c r="J104" s="10"/>
+      <c r="K104" s="10"/>
+      <c r="L104" s="10"/>
+      <c r="M104" s="10"/>
+    </row>
+    <row r="105" ht="20.05" customHeight="1">
+      <c r="A105" s="10"/>
+      <c r="B105" s="10"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10"/>
+      <c r="K105" s="10"/>
+      <c r="L105" s="10"/>
+      <c r="M105" s="10"/>
+    </row>
+    <row r="106" ht="20.05" customHeight="1">
+      <c r="A106" s="10"/>
+      <c r="B106" s="10"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="J106" s="10"/>
+      <c r="K106" s="10"/>
+      <c r="L106" s="10"/>
+      <c r="M106" s="10"/>
+    </row>
+    <row r="107" ht="20.05" customHeight="1">
+      <c r="A107" s="10"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
+      <c r="L107" s="10"/>
+      <c r="M107" s="10"/>
+    </row>
+    <row r="108" ht="20.05" customHeight="1">
+      <c r="A108" s="10"/>
+      <c r="B108" s="10"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="10"/>
+      <c r="J108" s="10"/>
+      <c r="K108" s="10"/>
+      <c r="L108" s="10"/>
+      <c r="M108" s="10"/>
+    </row>
+    <row r="109" ht="20.05" customHeight="1">
+      <c r="A109" s="10"/>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+      <c r="J109" s="10"/>
+      <c r="K109" s="10"/>
+      <c r="L109" s="10"/>
+      <c r="M109" s="10"/>
+    </row>
+    <row r="110" ht="20.05" customHeight="1">
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
+      <c r="G110" s="12"/>
+      <c r="H110" s="12"/>
+      <c r="I110" s="11"/>
+      <c r="J110" s="11"/>
+      <c r="K110" s="11"/>
+      <c r="L110" s="11"/>
+      <c r="M110" s="11"/>
+    </row>
+    <row r="111" ht="20.05" customHeight="1">
+      <c r="A111" s="11"/>
+      <c r="B111" s="11"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="12"/>
+      <c r="H111" s="12"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="11"/>
+      <c r="K111" s="11"/>
+      <c r="L111" s="11"/>
+      <c r="M111" s="11"/>
+    </row>
+    <row r="112" ht="20.05" customHeight="1">
+      <c r="A112" s="11"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
+      <c r="F112" s="12"/>
+      <c r="G112" s="12"/>
+      <c r="H112" s="12"/>
+      <c r="I112" s="11"/>
+      <c r="J112" s="11"/>
+      <c r="K112" s="11"/>
+      <c r="L112" s="11"/>
+      <c r="M112" s="11"/>
+    </row>
+    <row r="113" ht="20.05" customHeight="1">
+      <c r="A113" s="11"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
+      <c r="G113" s="12"/>
+      <c r="H113" s="12"/>
+      <c r="I113" s="11"/>
+      <c r="J113" s="11"/>
+      <c r="K113" s="11"/>
+      <c r="L113" s="11"/>
+      <c r="M113" s="11"/>
+    </row>
+    <row r="114" ht="20.05" customHeight="1">
+      <c r="A114" s="11"/>
+      <c r="B114" s="11"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="12"/>
+      <c r="H114" s="12"/>
+      <c r="I114" s="11"/>
+      <c r="J114" s="11"/>
+      <c r="K114" s="11"/>
+      <c r="L114" s="11"/>
+      <c r="M114" s="11"/>
+    </row>
+    <row r="115" ht="20.05" customHeight="1">
+      <c r="A115" s="11"/>
+      <c r="B115" s="11"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
+      <c r="G115" s="12"/>
+      <c r="H115" s="12"/>
+      <c r="I115" s="11"/>
+      <c r="J115" s="11"/>
+      <c r="K115" s="11"/>
+      <c r="L115" s="11"/>
+      <c r="M115" s="11"/>
+    </row>
+    <row r="116" ht="20.05" customHeight="1">
+      <c r="A116" s="11"/>
+      <c r="B116" s="11"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
+      <c r="G116" s="12"/>
+      <c r="H116" s="12"/>
+      <c r="I116" s="11"/>
+      <c r="J116" s="11"/>
+      <c r="K116" s="11"/>
+      <c r="L116" s="11"/>
+      <c r="M116" s="11"/>
+    </row>
+    <row r="117" ht="20.05" customHeight="1">
+      <c r="A117" s="11"/>
+      <c r="B117" s="11"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+      <c r="G117" s="12"/>
+      <c r="H117" s="12"/>
+      <c r="I117" s="11"/>
+      <c r="J117" s="11"/>
+      <c r="K117" s="11"/>
+      <c r="L117" s="11"/>
+      <c r="M117" s="11"/>
+    </row>
+    <row r="118" ht="20.05" customHeight="1">
+      <c r="A118" s="11"/>
+      <c r="B118" s="11"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="12"/>
+      <c r="G118" s="12"/>
+      <c r="H118" s="12"/>
+      <c r="I118" s="11"/>
+      <c r="J118" s="11"/>
+      <c r="K118" s="11"/>
+      <c r="L118" s="11"/>
+      <c r="M118" s="11"/>
+    </row>
+    <row r="119" ht="20.05" customHeight="1">
+      <c r="A119" s="11"/>
+      <c r="B119" s="11"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
+      <c r="G119" s="12"/>
+      <c r="H119" s="12"/>
+      <c r="I119" s="11"/>
+      <c r="J119" s="11"/>
+      <c r="K119" s="11"/>
+      <c r="L119" s="11"/>
+      <c r="M119" s="11"/>
+    </row>
+    <row r="120" ht="20.05" customHeight="1">
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+      <c r="H120" s="12"/>
+      <c r="I120" s="11"/>
+      <c r="J120" s="11"/>
+      <c r="K120" s="11"/>
+      <c r="L120" s="11"/>
+      <c r="M120" s="11"/>
+    </row>
+    <row r="121" ht="20.05" customHeight="1">
+      <c r="A121" s="11"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
+      <c r="G121" s="12"/>
+      <c r="H121" s="12"/>
+      <c r="I121" s="11"/>
+      <c r="J121" s="11"/>
+      <c r="K121" s="11"/>
+      <c r="L121" s="11"/>
+      <c r="M121" s="11"/>
+    </row>
+    <row r="122" ht="20.05" customHeight="1">
+      <c r="A122" s="11"/>
+      <c r="B122" s="11"/>
+      <c r="C122" s="12"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
+      <c r="F122" s="12"/>
+      <c r="G122" s="12"/>
+      <c r="H122" s="12"/>
+      <c r="I122" s="11"/>
+      <c r="J122" s="11"/>
+      <c r="K122" s="11"/>
+      <c r="L122" s="11"/>
+      <c r="M122" s="11"/>
+    </row>
+    <row r="123" ht="20.05" customHeight="1">
+      <c r="A123" s="11"/>
+      <c r="B123" s="11"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
+      <c r="G123" s="12"/>
+      <c r="H123" s="12"/>
+      <c r="I123" s="11"/>
+      <c r="J123" s="11"/>
+      <c r="K123" s="11"/>
+      <c r="L123" s="11"/>
+      <c r="M123" s="11"/>
+    </row>
+    <row r="124" ht="20.05" customHeight="1">
+      <c r="A124" s="11"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
+      <c r="G124" s="12"/>
+      <c r="H124" s="12"/>
+      <c r="I124" s="11"/>
+      <c r="J124" s="11"/>
+      <c r="K124" s="11"/>
+      <c r="L124" s="11"/>
+      <c r="M124" s="11"/>
+    </row>
+    <row r="125" ht="20.05" customHeight="1">
+      <c r="A125" s="11"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
+      <c r="G125" s="12"/>
+      <c r="H125" s="12"/>
+      <c r="I125" s="11"/>
+      <c r="J125" s="11"/>
+      <c r="K125" s="11"/>
+      <c r="L125" s="11"/>
+      <c r="M125" s="11"/>
+    </row>
+    <row r="126" ht="20.05" customHeight="1">
+      <c r="A126" s="11"/>
+      <c r="B126" s="11"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+      <c r="G126" s="12"/>
+      <c r="H126" s="12"/>
+      <c r="I126" s="11"/>
+      <c r="J126" s="11"/>
+      <c r="K126" s="11"/>
+      <c r="L126" s="11"/>
+      <c r="M126" s="11"/>
+    </row>
+    <row r="127" ht="20.05" customHeight="1">
+      <c r="A127" s="11"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+      <c r="G127" s="12"/>
+      <c r="H127" s="12"/>
+      <c r="I127" s="11"/>
+      <c r="J127" s="11"/>
+      <c r="K127" s="11"/>
+      <c r="L127" s="11"/>
+      <c r="M127" s="11"/>
+    </row>
+    <row r="128" ht="20.05" customHeight="1">
+      <c r="A128" s="11"/>
+      <c r="B128" s="11"/>
+      <c r="C128" s="12"/>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
+      <c r="F128" s="12"/>
+      <c r="G128" s="12"/>
+      <c r="H128" s="12"/>
+      <c r="I128" s="11"/>
+      <c r="J128" s="11"/>
+      <c r="K128" s="11"/>
+      <c r="L128" s="11"/>
+      <c r="M128" s="11"/>
+    </row>
+    <row r="129" ht="20.05" customHeight="1">
+      <c r="A129" s="11"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
+      <c r="F129" s="12"/>
+      <c r="G129" s="12"/>
+      <c r="H129" s="12"/>
+      <c r="I129" s="11"/>
+      <c r="J129" s="11"/>
+      <c r="K129" s="11"/>
+      <c r="L129" s="11"/>
+      <c r="M129" s="11"/>
+    </row>
+    <row r="130" ht="20.05" customHeight="1">
+      <c r="A130" s="11"/>
+      <c r="B130" s="11"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
+      <c r="F130" s="12"/>
+      <c r="G130" s="12"/>
+      <c r="H130" s="12"/>
+      <c r="I130" s="11"/>
+      <c r="J130" s="11"/>
+      <c r="K130" s="11"/>
+      <c r="L130" s="11"/>
+      <c r="M130" s="11"/>
+    </row>
+    <row r="131" ht="20.05" customHeight="1">
+      <c r="A131" s="11"/>
+      <c r="B131" s="11"/>
+      <c r="C131" s="12"/>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="12"/>
+      <c r="G131" s="12"/>
+      <c r="H131" s="12"/>
+      <c r="I131" s="11"/>
+      <c r="J131" s="11"/>
+      <c r="K131" s="11"/>
+      <c r="L131" s="11"/>
+      <c r="M131" s="11"/>
+    </row>
+    <row r="132" ht="20.05" customHeight="1">
+      <c r="A132" s="11"/>
+      <c r="B132" s="11"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12"/>
+      <c r="G132" s="12"/>
+      <c r="H132" s="12"/>
+      <c r="I132" s="11"/>
+      <c r="J132" s="11"/>
+      <c r="K132" s="11"/>
+      <c r="L132" s="11"/>
+      <c r="M132" s="11"/>
+    </row>
+    <row r="133" ht="20.05" customHeight="1">
+      <c r="A133" s="11"/>
+      <c r="B133" s="11"/>
+      <c r="C133" s="12"/>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12"/>
+      <c r="F133" s="12"/>
+      <c r="G133" s="12"/>
+      <c r="H133" s="12"/>
+      <c r="I133" s="11"/>
+      <c r="J133" s="11"/>
+      <c r="K133" s="11"/>
+      <c r="L133" s="11"/>
+      <c r="M133" s="11"/>
+    </row>
+    <row r="134" ht="20.05" customHeight="1">
+      <c r="A134" s="11"/>
+      <c r="B134" s="11"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
+      <c r="G134" s="12"/>
+      <c r="H134" s="12"/>
+      <c r="I134" s="11"/>
+      <c r="J134" s="11"/>
+      <c r="K134" s="11"/>
+      <c r="L134" s="11"/>
+      <c r="M134" s="11"/>
+    </row>
+    <row r="135" ht="20.05" customHeight="1">
+      <c r="A135" s="11"/>
+      <c r="B135" s="11"/>
+      <c r="C135" s="12"/>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
+      <c r="F135" s="12"/>
+      <c r="G135" s="12"/>
+      <c r="H135" s="12"/>
+      <c r="I135" s="11"/>
+      <c r="J135" s="11"/>
+      <c r="K135" s="11"/>
+      <c r="L135" s="11"/>
+      <c r="M135" s="11"/>
+    </row>
+    <row r="136" ht="20.05" customHeight="1">
+      <c r="A136" s="11"/>
+      <c r="B136" s="11"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12"/>
+      <c r="F136" s="12"/>
+      <c r="G136" s="12"/>
+      <c r="H136" s="12"/>
+      <c r="I136" s="11"/>
+      <c r="J136" s="11"/>
+      <c r="K136" s="11"/>
+      <c r="L136" s="11"/>
+      <c r="M136" s="11"/>
+    </row>
+    <row r="137" ht="20.05" customHeight="1">
+      <c r="A137" s="11"/>
+      <c r="B137" s="11"/>
+      <c r="C137" s="12"/>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="12"/>
+      <c r="G137" s="12"/>
+      <c r="H137" s="12"/>
+      <c r="I137" s="11"/>
+      <c r="J137" s="11"/>
+      <c r="K137" s="11"/>
+      <c r="L137" s="11"/>
+      <c r="M137" s="11"/>
+    </row>
+    <row r="138" ht="20.05" customHeight="1">
+      <c r="A138" s="11"/>
+      <c r="B138" s="11"/>
+      <c r="C138" s="12"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12"/>
+      <c r="F138" s="12"/>
+      <c r="G138" s="12"/>
+      <c r="H138" s="12"/>
+      <c r="I138" s="11"/>
+      <c r="J138" s="11"/>
+      <c r="K138" s="11"/>
+      <c r="L138" s="11"/>
+      <c r="M138" s="11"/>
+    </row>
+    <row r="139" ht="20.05" customHeight="1">
+      <c r="A139" s="11"/>
+      <c r="B139" s="11"/>
+      <c r="C139" s="12"/>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="12"/>
+      <c r="H139" s="12"/>
+      <c r="I139" s="11"/>
+      <c r="J139" s="11"/>
+      <c r="K139" s="11"/>
+      <c r="L139" s="11"/>
+      <c r="M139" s="11"/>
+    </row>
+    <row r="140" ht="20.05" customHeight="1">
+      <c r="A140" s="11"/>
+      <c r="B140" s="11"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="12"/>
+      <c r="E140" s="12"/>
+      <c r="F140" s="12"/>
+      <c r="G140" s="12"/>
+      <c r="H140" s="12"/>
+      <c r="I140" s="11"/>
+      <c r="J140" s="11"/>
+      <c r="K140" s="11"/>
+      <c r="L140" s="11"/>
+      <c r="M140" s="11"/>
+    </row>
+    <row r="141" ht="20.05" customHeight="1">
+      <c r="A141" s="11"/>
+      <c r="B141" s="11"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="12"/>
+      <c r="E141" s="12"/>
+      <c r="F141" s="12"/>
+      <c r="G141" s="12"/>
+      <c r="H141" s="12"/>
+      <c r="I141" s="11"/>
+      <c r="J141" s="11"/>
+      <c r="K141" s="11"/>
+      <c r="L141" s="11"/>
+      <c r="M141" s="11"/>
+    </row>
+    <row r="142" ht="20.05" customHeight="1">
+      <c r="A142" s="11"/>
+      <c r="B142" s="11"/>
+      <c r="C142" s="12"/>
+      <c r="D142" s="12"/>
+      <c r="E142" s="12"/>
+      <c r="F142" s="12"/>
+      <c r="G142" s="12"/>
+      <c r="H142" s="12"/>
+      <c r="I142" s="11"/>
+      <c r="J142" s="11"/>
+      <c r="K142" s="11"/>
+      <c r="L142" s="11"/>
+      <c r="M142" s="11"/>
+    </row>
+    <row r="143" ht="20.05" customHeight="1">
+      <c r="A143" s="11"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="12"/>
+      <c r="G143" s="12"/>
+      <c r="H143" s="12"/>
+      <c r="I143" s="11"/>
+      <c r="J143" s="11"/>
+      <c r="K143" s="11"/>
+      <c r="L143" s="11"/>
+      <c r="M143" s="11"/>
+    </row>
+    <row r="144" ht="20.05" customHeight="1">
+      <c r="A144" s="11"/>
+      <c r="B144" s="11"/>
+      <c r="C144" s="12"/>
+      <c r="D144" s="12"/>
+      <c r="E144" s="12"/>
+      <c r="F144" s="12"/>
+      <c r="G144" s="12"/>
+      <c r="H144" s="12"/>
+      <c r="I144" s="11"/>
+      <c r="J144" s="11"/>
+      <c r="K144" s="11"/>
+      <c r="L144" s="11"/>
+      <c r="M144" s="11"/>
+    </row>
+    <row r="145" ht="20.05" customHeight="1">
+      <c r="A145" s="11"/>
+      <c r="B145" s="11"/>
+      <c r="C145" s="12"/>
+      <c r="D145" s="12"/>
+      <c r="E145" s="12"/>
+      <c r="F145" s="12"/>
+      <c r="G145" s="12"/>
+      <c r="H145" s="12"/>
+      <c r="I145" s="11"/>
+      <c r="J145" s="11"/>
+      <c r="K145" s="11"/>
+      <c r="L145" s="11"/>
+      <c r="M145" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>